<commit_message>
Got terrible results from using the new IF, also fixed the more_data file back to before klp and klinflux were taken out
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox_moredata.xlsx
+++ b/Lacex_summary_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37428456-F6B8-42BE-A894-A47490364A9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18DDD94-C812-4891-8094-118019DEB6B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A183822-7954-4BE4-BDAB-B5FAE4C8B5A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A183822-7954-4BE4-BDAB-B5FAE4C8B5A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,16 +831,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.4394371902156326E-4</c:v>
+                    <c:v>1.4110540454517E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1454985630101012E-3</c:v>
+                    <c:v>1.1938388220454957E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0252324897493665E-2</c:v>
+                    <c:v>1.0219978638120604E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.2710599724978308E-4</c:v>
+                    <c:v>4.2920729768569356E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -852,16 +852,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.4394371902156326E-4</c:v>
+                    <c:v>1.4110540454517E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1454985630101012E-3</c:v>
+                    <c:v>1.1938388220454957E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0252324897493665E-2</c:v>
+                    <c:v>1.0219978638120604E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.2710599724978308E-4</c:v>
+                    <c:v>4.2920729768569356E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -907,16 +907,16 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.3164158690311869E-3</c:v>
+                  <c:v>2.3173268963984188E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3841099779699843E-3</c:v>
+                  <c:v>6.5132119631182801E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7259684965693379E-2</c:v>
+                  <c:v>2.7535106283079838E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9438179583043522E-3</c:v>
+                  <c:v>5.0273961825241173E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1185,16 +1185,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.0119091447892565E-2</c:v>
+                    <c:v>1.2057455739979463E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.4093217675224937E-2</c:v>
+                    <c:v>5.7309495294150879E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.39819613118576136</c:v>
+                    <c:v>0.39928208436858398</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.14503347676822781</c:v>
+                    <c:v>0.13741088889033834</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1206,16 +1206,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.0119091447892565E-2</c:v>
+                    <c:v>1.2057455739979463E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.4093217675224937E-2</c:v>
+                    <c:v>5.7309495294150879E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.39819613118576136</c:v>
+                    <c:v>0.39928208436858398</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.14503347676822781</c:v>
+                    <c:v>0.13741088889033834</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1261,16 +1261,16 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.1562026481064915E-2</c:v>
+                  <c:v>9.2535545750464687E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35224348703388203</c:v>
+                  <c:v>0.3541415185008206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74774420072208381</c:v>
+                  <c:v>0.75444268232926348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17801503044574071</c:v>
+                  <c:v>0.16916415025152015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1539,19 +1539,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.4510193064883369E-2</c:v>
+                    <c:v>2.3803754511435734E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.4560951831086825E-2</c:v>
+                    <c:v>2.3947765296666392E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.117040559412727E-2</c:v>
+                    <c:v>1.0466686942143609E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5218377435181186E-2</c:v>
+                    <c:v>1.4625933793160245E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.2305776623275939E-8</c:v>
+                    <c:v>6.9919142025448567E-7</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1563,19 +1563,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>2.4510193064883369E-2</c:v>
+                    <c:v>2.3803754511435734E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.4560951831086825E-2</c:v>
+                    <c:v>2.3947765296666392E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.117040559412727E-2</c:v>
+                    <c:v>1.0466686942143609E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5218377435181186E-2</c:v>
+                    <c:v>1.4625933793160245E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.2305776623275939E-8</c:v>
+                    <c:v>6.9919142025448567E-7</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1627,22 +1627,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.5338792243522842E-2</c:v>
+                  <c:v>7.384890314233869E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0878096231398669E-2</c:v>
+                  <c:v>5.0263555960985945E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9605294490649968E-2</c:v>
+                  <c:v>6.3109847044927683E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5438489871608422E-2</c:v>
+                  <c:v>8.0357873156810505E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9996154785638877E-2</c:v>
+                  <c:v>9.9999999990512817E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9999611247921769E-2</c:v>
+                  <c:v>9.9999300808557345E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1911,19 +1911,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.8905919800278743E-4</c:v>
+                    <c:v>3.8194997275177109E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.0506651067963139E-4</c:v>
+                    <c:v>2.9494907968756836E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.1590559082891949E-4</c:v>
+                    <c:v>2.310682053692697E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.6278990617203001E-4</c:v>
+                    <c:v>4.7544596282562859E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>9.8987882803977523E-5</c:v>
+                    <c:v>1.7933404971992757E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1935,19 +1935,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.8905919800278743E-4</c:v>
+                    <c:v>3.8194997275177109E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.0506651067963139E-4</c:v>
+                    <c:v>2.9494907968756836E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.1590559082891949E-4</c:v>
+                    <c:v>2.310682053692697E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.6278990617203001E-4</c:v>
+                    <c:v>4.7544596282562859E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>9.8987882803977523E-5</c:v>
+                    <c:v>1.7933404971992757E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1999,22 +1999,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.037862058825092E-2</c:v>
+                  <c:v>2.0365681512952261E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9912909647962457E-2</c:v>
+                  <c:v>1.9902792231451975E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0515103427541762E-2</c:v>
+                  <c:v>2.0561912508965351E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0409427432635803E-2</c:v>
+                  <c:v>2.0431830067845134E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0902529677286813E-2</c:v>
+                  <c:v>2.0784713283118691E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.068643633958234E-2</c:v>
+                  <c:v>2.0754795921728013E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2283,19 +2283,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.790444705159948E-5</c:v>
+                    <c:v>2.1625069528551808E-5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.4724977136014664E-5</c:v>
+                    <c:v>4.8710360305349656E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.6268316449898223E-4</c:v>
+                    <c:v>1.614486351023254E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9335632166111503E-4</c:v>
+                    <c:v>1.279616788292203E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.7860731561090558E-6</c:v>
+                    <c:v>2.9679016567189798E-5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2307,19 +2307,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.790444705159948E-5</c:v>
+                    <c:v>2.1625069528551808E-5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.4724977136014664E-5</c:v>
+                    <c:v>4.8710360305349656E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.6268316449898223E-4</c:v>
+                    <c:v>1.614486351023254E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9335632166111503E-4</c:v>
+                    <c:v>1.279616788292203E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.7860731561090558E-6</c:v>
+                    <c:v>2.9679016567189798E-5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2371,22 +2371,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.6626665084659509E-2</c:v>
+                  <c:v>2.6578997644427605E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.678220265577928E-2</c:v>
+                  <c:v>2.6835872828472173E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6913361518582011E-2</c:v>
+                  <c:v>2.6886662268571313E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6763462286901768E-2</c:v>
+                  <c:v>2.6657237171290454E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6623766806585347E-2</c:v>
+                  <c:v>2.6593421852223683E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6746041579962625E-2</c:v>
+                  <c:v>2.6777762541119757E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,19 +2655,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>1.4394371902156326E-4</c:v>
+                    <c:v>1.4110540454517E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1454985630101012E-3</c:v>
+                    <c:v>1.1938388220454957E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0252324897493665E-2</c:v>
+                    <c:v>1.0219978638120604E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.2710599724978308E-4</c:v>
+                    <c:v>4.2920729768569356E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1447888678808326E-4</c:v>
+                    <c:v>4.7600411383151179E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2679,19 +2679,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>1.4394371902156326E-4</c:v>
+                    <c:v>1.4110540454517E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1454985630101012E-3</c:v>
+                    <c:v>1.1938388220454957E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0252324897493665E-2</c:v>
+                    <c:v>1.0219978638120604E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.2710599724978308E-4</c:v>
+                    <c:v>4.2920729768569356E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1447888678808326E-4</c:v>
+                    <c:v>4.7600411383151179E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2743,22 +2743,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.3164158690311869E-3</c:v>
+                  <c:v>2.3173268963984188E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3841099779699843E-3</c:v>
+                  <c:v>6.5132119631182801E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7259684965693379E-2</c:v>
+                  <c:v>2.7535106283079838E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9438179583043522E-3</c:v>
+                  <c:v>5.0273961825241173E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0575516431258088E-2</c:v>
+                  <c:v>1.0760566128758033E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.1513467267411528E-3</c:v>
+                  <c:v>7.218428100833273E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3027,19 +3027,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>1.0119091447892565E-2</c:v>
+                    <c:v>1.2057455739979463E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.4093217675224937E-2</c:v>
+                    <c:v>5.7309495294150879E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.39819613118576136</c:v>
+                    <c:v>0.39928208436858398</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.14503347676822781</c:v>
+                    <c:v>0.13741088889033834</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.6027079767790373E-2</c:v>
+                    <c:v>1.8308667441519141E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3051,19 +3051,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>1.0119091447892565E-2</c:v>
+                    <c:v>1.2057455739979463E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.4093217675224937E-2</c:v>
+                    <c:v>5.7309495294150879E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.39819613118576136</c:v>
+                    <c:v>0.39928208436858398</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.14503347676822781</c:v>
+                    <c:v>0.13741088889033834</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.6027079767790373E-2</c:v>
+                    <c:v>1.8308667441519141E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3115,22 +3115,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.1562026481064915E-2</c:v>
+                  <c:v>9.2535545750464687E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35224348703388203</c:v>
+                  <c:v>0.3541415185008206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74774420072208381</c:v>
+                  <c:v>0.75444268232926348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17801503044574071</c:v>
+                  <c:v>0.16916415025152015</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11351920357952909</c:v>
+                  <c:v>0.10810136923207164</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20672336535200575</c:v>
+                  <c:v>0.2047343855353021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3258,301 +3258,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="464000488"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$I$51:$N$51</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>HK-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>UMRC6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>UOK262</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>UOK + DIDS</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>siRNA_c</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>siRNA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$52:$N$52</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.8181824203370934E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.20297707272718515</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6671523445758363</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.79229808016207393</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.12935499209510501</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16609778493771393</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E020-4B75-A36C-FAD94D1D1009}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="586836440"/>
-        <c:axId val="586839720"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="586836440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="586839720"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="586839720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="586836440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3888,46 +3593,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6947,509 +6612,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8201,42 +7363,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>394447</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>35859</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>143436</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{043A2BEE-3832-43AC-8DB4-516492F6A41F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8545,8 +7671,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51:N52"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8558,282 +7684,282 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>2.0557108197518685E-3</v>
+        <v>2.0440913622746353E-3</v>
       </c>
       <c r="B1" s="2">
-        <v>9.9115865834907793E-2</v>
+        <v>0.10465567845805716</v>
       </c>
       <c r="C1" s="2">
-        <v>2.6318593651669588E-2</v>
+        <v>2.6315789473742499E-2</v>
       </c>
       <c r="D1" s="2">
-        <v>818926475.2901206</v>
+        <v>818926518.32173777</v>
       </c>
       <c r="E1" s="2">
-        <v>23.825886019786932</v>
+        <v>23.82609736019262</v>
       </c>
       <c r="F1" s="2">
-        <v>61.845609767826666</v>
+        <v>61.845367692256538</v>
       </c>
       <c r="G1" s="2">
-        <v>0.68881158557416244</v>
+        <v>0.68884824364616704</v>
       </c>
       <c r="H1" s="2">
-        <v>7.047740592792108E-2</v>
+        <v>6.8689081548227338E-2</v>
       </c>
       <c r="I1" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999999999777905E-3</v>
       </c>
       <c r="J1" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.2257708635855453E-14</v>
       </c>
       <c r="K1" s="2">
-        <v>0.99150334142583507</v>
+        <v>0.99150334140232921</v>
       </c>
       <c r="L1" s="2">
-        <v>0.98386808311956486</v>
+        <v>0.98468620622725533</v>
       </c>
       <c r="M1" s="2">
-        <v>0.9684973582343599</v>
+        <v>0.96903400881054969</v>
       </c>
       <c r="N1" s="2">
-        <v>9.171527674506165E-2</v>
+        <v>9.1715276871926474E-2</v>
       </c>
       <c r="O1" s="2">
-        <v>0.12637483021405344</v>
+        <v>0.12312861501299061</v>
       </c>
       <c r="P1" s="2">
-        <v>0.17660015670430126</v>
+        <v>0.17508949505197574</v>
       </c>
       <c r="Q1" s="2">
-        <v>2.0856355236519776E-2</v>
+        <v>2.0833159094342264E-2</v>
       </c>
       <c r="R1" s="2">
-        <v>2.6761929438158409E-2</v>
+        <v>2.6617079497839362E-2</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>2.3410137687248072E-3</v>
+        <v>2.3927976051121252E-3</v>
       </c>
       <c r="B2" s="2">
-        <v>0.10404526265993677</v>
+        <v>0.10453021573169838</v>
       </c>
       <c r="C2" s="2">
-        <v>9.9731461794397874E-2</v>
+        <v>9.5311438438472257E-2</v>
       </c>
       <c r="D2" s="2">
-        <v>36106164.569166452</v>
+        <v>36088455.454467326</v>
       </c>
       <c r="E2" s="2">
-        <v>18.681233832701423</v>
+        <v>18.681938922510028</v>
       </c>
       <c r="F2" s="2">
-        <v>58.210819368549934</v>
+        <v>58.195976647332117</v>
       </c>
       <c r="G2" s="2">
-        <v>1.0000022204460493E-8</v>
+        <v>2.9227470395530482E-6</v>
       </c>
       <c r="H2" s="2">
-        <v>2.6538587856825991E-2</v>
+        <v>2.7168577155675049E-2</v>
       </c>
       <c r="I2" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>5.4853470340308853E-14</v>
       </c>
       <c r="J2" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.7951610168121699E-3</v>
       </c>
       <c r="K2" s="2">
-        <v>0.99654307584778179</v>
+        <v>0.99654313831679786</v>
       </c>
       <c r="L2" s="2">
-        <v>0.98053574802914201</v>
+        <v>0.98089961043097618</v>
       </c>
       <c r="M2" s="2">
-        <v>0.99425352788773635</v>
+        <v>0.99419710437208608</v>
       </c>
       <c r="N2" s="2">
-        <v>5.8500896665744137E-2</v>
+        <v>5.8500368087475212E-2</v>
       </c>
       <c r="O2" s="2">
-        <v>0.13881501882415118</v>
+        <v>0.13751140197573994</v>
       </c>
       <c r="P2" s="2">
-        <v>7.5425508888843515E-2</v>
+        <v>7.5794898717755591E-2</v>
       </c>
       <c r="Q2" s="2">
-        <v>1.9607843137277106E-2</v>
+        <v>1.9608725866423513E-2</v>
       </c>
       <c r="R2" s="2">
-        <v>2.6569554684972144E-2</v>
+        <v>2.6577712286619641E-2</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2.5525230186168851E-3</v>
+        <v>2.5150917218084955E-3</v>
       </c>
       <c r="B3" s="2">
-        <v>7.1524950948350138E-2</v>
+        <v>6.8420743061638548E-2</v>
       </c>
       <c r="C3" s="2">
-        <v>9.9966321284501045E-2</v>
+        <v>9.9919481514801317E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>1041003656.6408843</v>
+        <v>1041012019.8025222</v>
       </c>
       <c r="E3" s="2">
-        <v>19.199045618070105</v>
+        <v>19.19905848943559</v>
       </c>
       <c r="F3" s="2">
-        <v>68.746358124488609</v>
+        <v>68.746258055837359</v>
       </c>
       <c r="G3" s="2">
-        <v>0.60200460717787152</v>
+        <v>0.60206471914450987</v>
       </c>
       <c r="H3" s="2">
-        <v>1.7529478825365742E-2</v>
+        <v>1.3162386949168365E-2</v>
       </c>
       <c r="I3" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>2.9701056386062662E-7</v>
       </c>
       <c r="J3" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>6.9695614230316312E-9</v>
       </c>
       <c r="K3" s="2">
-        <v>0.99165914575692848</v>
+        <v>0.99165914719180515</v>
       </c>
       <c r="L3" s="2">
-        <v>0.98348704836666767</v>
+        <v>0.98342962178459059</v>
       </c>
       <c r="M3" s="2">
-        <v>0.99316820740064393</v>
+        <v>0.99356881462323687</v>
       </c>
       <c r="N3" s="2">
-        <v>9.0870488612314851E-2</v>
+        <v>9.0870480796092098E-2</v>
       </c>
       <c r="O3" s="2">
-        <v>0.12785860204538047</v>
+        <v>0.12808073404402126</v>
       </c>
       <c r="P3" s="2">
-        <v>8.2240346991987581E-2</v>
+        <v>7.9792690912110151E-2</v>
       </c>
       <c r="Q3" s="2">
-        <v>2.0671663390955875E-2</v>
+        <v>2.0655159578091005E-2</v>
       </c>
       <c r="R3" s="2">
-        <v>2.6548511130847979E-2</v>
+        <v>2.6542201148823823E-2</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>5.2573198946346388E-3</v>
+        <v>5.3762528274266495E-3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.2859338949845297</v>
+        <v>0.28353888576952746</v>
       </c>
       <c r="C4" s="2">
-        <v>2.6318492905989185E-2</v>
+        <v>2.6315791785633313E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>86629034.117601648</v>
+        <v>86596842.841015711</v>
       </c>
       <c r="E4" s="2">
-        <v>30.913402420885536</v>
+        <v>30.913689726992203</v>
       </c>
       <c r="F4" s="2">
-        <v>58.043429814323368</v>
+        <v>58.032491918073021</v>
       </c>
       <c r="G4" s="2">
-        <v>1.0000033601550099E-8</v>
+        <v>1.0000054897723946E-8</v>
       </c>
       <c r="H4" s="2">
-        <v>0.19701764756584852</v>
+        <v>0.19489217419388372</v>
       </c>
       <c r="I4" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.5781641433140845E-7</v>
       </c>
       <c r="J4" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999999999661453E-3</v>
       </c>
       <c r="K4" s="2">
-        <v>0.99355644913506469</v>
+        <v>0.99355664494107587</v>
       </c>
       <c r="L4" s="2">
-        <v>0.93529759124292899</v>
+        <v>0.93629390894292164</v>
       </c>
       <c r="M4" s="2">
-        <v>0.9363863404679561</v>
+        <v>0.93686960382096918</v>
       </c>
       <c r="N4" s="2">
-        <v>7.9869364316275268E-2</v>
+        <v>7.9868150775730701E-2</v>
       </c>
       <c r="O4" s="2">
-        <v>0.25309165270609046</v>
+        <v>0.25113548165583355</v>
       </c>
       <c r="P4" s="2">
-        <v>0.25095322858398028</v>
+        <v>0.24999818442788838</v>
       </c>
       <c r="Q4" s="2">
-        <v>1.9607843137288503E-2</v>
+        <v>1.9607843137278452E-2</v>
       </c>
       <c r="R4" s="2">
-        <v>2.6749809655083442E-2</v>
+        <v>2.6896859532853503E-2</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>5.2200042368165719E-3</v>
+        <v>5.2633828822758588E-3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.45942873015341307</v>
+        <v>0.46763865279280215</v>
       </c>
       <c r="C5" s="2">
-        <v>9.9999999868893116E-2</v>
+        <v>9.8159086554318709E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>1103374597.4011326</v>
+        <v>1103368290.1447656</v>
       </c>
       <c r="E5" s="2">
-        <v>12.198208080747904</v>
+        <v>12.198015708622073</v>
       </c>
       <c r="F5" s="2">
-        <v>70.612985794234618</v>
+        <v>70.613225370925008</v>
       </c>
       <c r="G5" s="2">
-        <v>0.58520909191220483</v>
+        <v>0.58519336522215837</v>
       </c>
       <c r="H5" s="2">
-        <v>0.28420115416857</v>
+        <v>0.28961327237140227</v>
       </c>
       <c r="I5" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.0641221838503477E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.0084863790427543E-4</v>
       </c>
       <c r="K5" s="2">
-        <v>0.99461539023777035</v>
+        <v>0.99461538917933912</v>
       </c>
       <c r="L5" s="2">
-        <v>0.97094393467439111</v>
+        <v>0.97097659833260552</v>
       </c>
       <c r="M5" s="2">
-        <v>0.98152731522893832</v>
+        <v>0.98146415872607196</v>
       </c>
       <c r="N5" s="2">
-        <v>7.3012078895258084E-2</v>
+        <v>7.3012086071104015E-2</v>
       </c>
       <c r="O5" s="2">
-        <v>0.16960396419999402</v>
+        <v>0.16950860642079654</v>
       </c>
       <c r="P5" s="2">
-        <v>0.13523297646414142</v>
+        <v>0.1354639541028857</v>
       </c>
       <c r="Q5" s="2">
-        <v>2.0523042669321721E-2</v>
+        <v>2.0492690390827111E-2</v>
       </c>
       <c r="R5" s="2">
-        <v>2.6924749806119089E-2</v>
+        <v>2.6871171299631819E-2</v>
       </c>
       <c r="T5">
         <f>0.0001</f>
@@ -8883,58 +8009,58 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>8.6750058024587431E-3</v>
+        <v>8.9000001796523294E-3</v>
       </c>
       <c r="B6" s="2">
-        <v>0.31136783596370343</v>
+        <v>0.31124701694013229</v>
       </c>
       <c r="C6" s="2">
-        <v>2.6315795919313722E-2</v>
+        <v>2.631578954300581E-2</v>
       </c>
       <c r="D6" s="2">
-        <v>98184079.682801247</v>
+        <v>98184377.42764622</v>
       </c>
       <c r="E6" s="2">
-        <v>23.116385117845365</v>
+        <v>23.117265872845241</v>
       </c>
       <c r="F6" s="2">
-        <v>54.511981949431565</v>
+        <v>54.503896415532829</v>
       </c>
       <c r="G6" s="2">
-        <v>1.0000022247938887E-8</v>
+        <v>2.5048537685972825E-8</v>
       </c>
       <c r="H6" s="2">
-        <v>0.12771241644713691</v>
+        <v>0.12760821953460458</v>
       </c>
       <c r="I6" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.3713746761796656E-14</v>
       </c>
       <c r="J6" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.999999999976656E-3</v>
       </c>
       <c r="K6" s="2">
-        <v>0.99563273473730507</v>
+        <v>0.995632606519402</v>
       </c>
       <c r="L6" s="2">
-        <v>0.98648971431173471</v>
+        <v>0.98684403444459123</v>
       </c>
       <c r="M6" s="2">
-        <v>0.98965810503377805</v>
+        <v>0.98980638844998814</v>
       </c>
       <c r="N6" s="2">
-        <v>6.5754031131695631E-2</v>
+        <v>6.5754996356109957E-2</v>
       </c>
       <c r="O6" s="2">
-        <v>0.11565112550849928</v>
+        <v>0.11412451927545925</v>
       </c>
       <c r="P6" s="2">
-        <v>0.10118535475334206</v>
+        <v>0.1004573314124549</v>
       </c>
       <c r="Q6" s="2">
-        <v>1.9607843137277151E-2</v>
+        <v>1.9607843166250361E-2</v>
       </c>
       <c r="R6" s="2">
-        <v>2.6672048506135308E-2</v>
+        <v>2.673958765293119E-2</v>
       </c>
       <c r="T6">
         <v>0.08</v>
@@ -8980,674 +8106,674 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>7.5914217578140148E-3</v>
+        <v>7.8104063053251026E-3</v>
       </c>
       <c r="B7" s="2">
-        <v>5.927771422376648E-2</v>
+        <v>5.8711767021941051E-2</v>
       </c>
       <c r="C7" s="2">
-        <v>2.6751329841161617E-2</v>
+        <v>3.543964728375152E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>869265109.56504738</v>
+        <v>869498093.87442935</v>
       </c>
       <c r="E7" s="2">
-        <v>39.084775814154654</v>
+        <v>39.085223327586924</v>
       </c>
       <c r="F7" s="2">
-        <v>54.55953109716026</v>
+        <v>54.559074477882291</v>
       </c>
       <c r="G7" s="2">
-        <v>0.80286497743261798</v>
+        <v>0.80289228249175082</v>
       </c>
       <c r="H7" s="2">
-        <v>5.9185138442204535E-2</v>
+        <v>4.7854248498612514E-2</v>
       </c>
       <c r="I7" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999986481246975E-3</v>
       </c>
       <c r="J7" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>2.4603233390046519E-10</v>
       </c>
       <c r="K7" s="2">
-        <v>0.99705611110648651</v>
+        <v>0.99705613162044915</v>
       </c>
       <c r="L7" s="2">
-        <v>0.99608504897129768</v>
+        <v>0.99612595656099368</v>
       </c>
       <c r="M7" s="2">
-        <v>0.99607006071385595</v>
+        <v>0.9962224675360567</v>
       </c>
       <c r="N7" s="2">
-        <v>5.3985646282863058E-2</v>
+        <v>5.3985458187879524E-2</v>
       </c>
       <c r="O7" s="2">
-        <v>6.2255935607902234E-2</v>
+        <v>6.1929823224487417E-2</v>
       </c>
       <c r="P7" s="2">
-        <v>6.2374994134529668E-2</v>
+        <v>6.1153553774935428E-2</v>
       </c>
       <c r="Q7" s="2">
-        <v>2.1232063794185255E-2</v>
+        <v>2.1219783761821043E-2</v>
       </c>
       <c r="R7" s="2">
-        <v>2.6553018643162851E-2</v>
+        <v>2.6547519541939579E-2</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1.0292223770819856E-2</v>
+        <v>1.0293977888170207E-2</v>
       </c>
       <c r="B8" s="2">
-        <v>6.2536956357797657E-2</v>
+        <v>6.2547230470345092E-2</v>
       </c>
       <c r="C8" s="2">
-        <v>9.9999470913624322E-2</v>
+        <v>9.9999997394403309E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>1105943154.5792081</v>
+        <v>1105943837.1576962</v>
       </c>
       <c r="E8" s="2">
-        <v>34.224739942760991</v>
+        <v>34.224737105350428</v>
       </c>
       <c r="F8" s="2">
-        <v>62.585366069851858</v>
+        <v>62.585373087947318</v>
       </c>
       <c r="G8" s="2">
-        <v>0.66656970850361874</v>
+        <v>0.66678525636758301</v>
       </c>
       <c r="H8" s="2">
-        <v>7.9010518088754811E-2</v>
+        <v>7.9059354392826436E-2</v>
       </c>
       <c r="I8" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>5.0899272976990542E-7</v>
       </c>
       <c r="J8" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>2.0085230956227377E-8</v>
       </c>
       <c r="K8" s="2">
-        <v>0.9974871711289971</v>
+        <v>0.99748717120289465</v>
       </c>
       <c r="L8" s="2">
-        <v>0.99501433922147275</v>
+        <v>0.99501466113717596</v>
       </c>
       <c r="M8" s="2">
-        <v>0.99238741847950507</v>
+        <v>0.99238547744077443</v>
       </c>
       <c r="N8" s="2">
-        <v>4.9879348203746052E-2</v>
+        <v>4.9879347470318032E-2</v>
       </c>
       <c r="O8" s="2">
-        <v>7.0258791624407971E-2</v>
+        <v>7.0256523341985691E-2</v>
       </c>
       <c r="P8" s="2">
-        <v>8.6817103304778445E-2</v>
+        <v>8.6828170813152195E-2</v>
       </c>
       <c r="Q8" s="2">
-        <v>2.0827320197030003E-2</v>
+        <v>2.0609537938434234E-2</v>
       </c>
       <c r="R8" s="2">
-        <v>2.6734421910361135E-2</v>
+        <v>2.6714034551213846E-2</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>2.5438395272100494E-2</v>
+        <v>2.5521490650557456E-2</v>
       </c>
       <c r="B9" s="2">
-        <v>3.4276101219153241</v>
+        <v>3.417715349211504</v>
       </c>
       <c r="C9" s="2">
-        <v>4.0395763664708331E-2</v>
+        <v>5.2458562678055182E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>488710735.85129702</v>
+        <v>489736763.11978352</v>
       </c>
       <c r="E9" s="2">
-        <v>29.4323485220031</v>
+        <v>29.439042175107609</v>
       </c>
       <c r="F9" s="2">
-        <v>66.759922800315707</v>
+        <v>66.768414906688562</v>
       </c>
       <c r="G9" s="2">
-        <v>5.7356304864502765E-2</v>
+        <v>5.7674886716178216E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>9.993133311341456</v>
+        <v>9.9656548726176819</v>
       </c>
       <c r="I9" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>4.6822527483963297E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.6097395522457985E-3</v>
       </c>
       <c r="K9" s="2">
-        <v>0.99576792369621603</v>
+        <v>0.99576792146742721</v>
       </c>
       <c r="L9" s="2">
-        <v>0.938327355439035</v>
+        <v>0.93833622632773017</v>
       </c>
       <c r="M9" s="2">
-        <v>0.97354796686243017</v>
+        <v>0.97355014251882899</v>
       </c>
       <c r="N9" s="2">
-        <v>6.4728321009787509E-2</v>
+        <v>6.4728338054109727E-2</v>
       </c>
       <c r="O9" s="2">
-        <v>0.2470949576890539</v>
+        <v>0.24707718618995786</v>
       </c>
       <c r="P9" s="2">
-        <v>0.16182556289472361</v>
+        <v>0.1618189077529549</v>
       </c>
       <c r="Q9" s="2">
-        <v>1.9857743757391303E-2</v>
+        <v>1.9839079069671032E-2</v>
       </c>
       <c r="R9" s="2">
-        <v>2.7489220908451125E-2</v>
+        <v>2.7391887592862471E-2</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>2.8744849719548491E-3</v>
+        <v>3.146457105211109E-3</v>
       </c>
       <c r="B10" s="2">
-        <v>0.32143880300750538</v>
+        <v>0.30767357664672129</v>
       </c>
       <c r="C10" s="2">
-        <v>2.6714907621898286E-2</v>
+        <v>7.9583445150516172E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>61788946.500900015</v>
+        <v>61731100.736689009</v>
       </c>
       <c r="E10" s="2">
-        <v>37.504357344146641</v>
+        <v>37.500782638502137</v>
       </c>
       <c r="F10" s="2">
-        <v>39.890323955715708</v>
+        <v>39.883935665374395</v>
       </c>
       <c r="G10" s="2">
-        <v>2.9917140721475569E-2</v>
+        <v>2.9511046557444614E-2</v>
       </c>
       <c r="H10" s="2">
-        <v>0.29137609880857473</v>
+        <v>0.27047908843108182</v>
       </c>
       <c r="I10" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>4.8746249878534728E-3</v>
       </c>
       <c r="J10" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.395798534112733E-3</v>
       </c>
       <c r="K10" s="2">
-        <v>0.99451207342539116</v>
+        <v>0.99451203358238027</v>
       </c>
       <c r="L10" s="2">
-        <v>0.98275643506478261</v>
+        <v>0.98442477385521798</v>
       </c>
       <c r="M10" s="2">
-        <v>0.99120152697749986</v>
+        <v>0.99115715378663338</v>
       </c>
       <c r="N10" s="2">
-        <v>7.3709207761735743E-2</v>
+        <v>7.3709475330133459E-2</v>
       </c>
       <c r="O10" s="2">
-        <v>0.13065653173823807</v>
+        <v>0.12417517418282223</v>
       </c>
       <c r="P10" s="2">
-        <v>9.3329996744214799E-2</v>
+        <v>9.356504556314281E-2</v>
       </c>
       <c r="Q10" s="2">
-        <v>1.9665017824744974E-2</v>
+        <v>1.9711737929038364E-2</v>
       </c>
       <c r="R10" s="2">
-        <v>2.6792616772375315E-2</v>
+        <v>2.6756523344968534E-2</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>8.5968463448288825E-3</v>
+        <v>8.6133116110997613E-3</v>
       </c>
       <c r="B11" s="2">
-        <v>7.5564336395165743E-2</v>
+        <v>7.5490511028491469E-2</v>
       </c>
       <c r="C11" s="2">
-        <v>4.0847045394112963E-2</v>
+        <v>4.1286898867914264E-2</v>
       </c>
       <c r="D11" s="2">
-        <v>110488423.18341053</v>
+        <v>110376839.87821494</v>
       </c>
       <c r="E11" s="2">
-        <v>18.841009981111771</v>
+        <v>18.842232094206679</v>
       </c>
       <c r="F11" s="2">
-        <v>71.952728345955066</v>
+        <v>71.952100802675602</v>
       </c>
       <c r="G11" s="2">
-        <v>0.61733761249913699</v>
+        <v>0.61663893787010804</v>
       </c>
       <c r="H11" s="2">
-        <v>9.8352057278380256E-2</v>
+        <v>9.8010561447073249E-2</v>
       </c>
       <c r="I11" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.3985244766235262E-4</v>
       </c>
       <c r="J11" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.4615726410125156E-9</v>
       </c>
       <c r="K11" s="2">
-        <v>0.98377987501298503</v>
+        <v>0.98377972734109542</v>
       </c>
       <c r="L11" s="2">
-        <v>0.98268451190627826</v>
+        <v>0.98268498828409034</v>
       </c>
       <c r="M11" s="2">
-        <v>0.98190575803062075</v>
+        <v>0.98190495840619718</v>
       </c>
       <c r="N11" s="2">
-        <v>0.12671986323045345</v>
+        <v>0.12672044007308195</v>
       </c>
       <c r="O11" s="2">
-        <v>0.13092873333529403</v>
+        <v>0.13092693228954302</v>
       </c>
       <c r="P11" s="2">
-        <v>0.13384057512460656</v>
+        <v>0.13384353244690153</v>
       </c>
       <c r="Q11" s="2">
-        <v>2.126960492623493E-2</v>
+        <v>2.1265776496996937E-2</v>
       </c>
       <c r="R11" s="2">
-        <v>2.6709984779518327E-2</v>
+        <v>2.6659677306561914E-2</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>7.9997766628592509E-2</v>
+        <v>7.9998621646789378E-2</v>
       </c>
       <c r="B12" s="2">
-        <v>2.0858082647647862</v>
+        <v>2.1312262426398703</v>
       </c>
       <c r="C12" s="2">
-        <v>7.9039145039425426E-2</v>
+        <v>3.3565295393196776E-2</v>
       </c>
       <c r="D12" s="2">
-        <v>1451043694.4494283</v>
+        <v>1451043698.7152901</v>
       </c>
       <c r="E12" s="2">
-        <v>12.000000000916236</v>
+        <v>12.000000000081066</v>
       </c>
       <c r="F12" s="2">
-        <v>77.207633189122404</v>
+        <v>77.207645232726918</v>
       </c>
       <c r="G12" s="2">
-        <v>0.44739495069051716</v>
+        <v>0.44746338058923973</v>
       </c>
       <c r="H12" s="2">
-        <v>4.1276322979465823</v>
+        <v>4.2189544038400131</v>
       </c>
       <c r="I12" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.0445275917702612E-3</v>
       </c>
       <c r="J12" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>4.2707190817022586E-14</v>
       </c>
       <c r="K12" s="2">
-        <v>0.96577834188396927</v>
+        <v>0.96577834202883539</v>
       </c>
       <c r="L12" s="2">
-        <v>0.93034998531482005</v>
+        <v>0.93034953850650604</v>
       </c>
       <c r="M12" s="2">
-        <v>0.9871643461549835</v>
+        <v>0.9871713206559789</v>
       </c>
       <c r="N12" s="2">
-        <v>0.1840636888005627</v>
+        <v>0.1840636884109762</v>
       </c>
       <c r="O12" s="2">
-        <v>0.2625900122592788</v>
+        <v>0.26259085452193304</v>
       </c>
       <c r="P12" s="2">
-        <v>0.11272664860877547</v>
+        <v>0.11269601834395418</v>
       </c>
       <c r="Q12" s="2">
-        <v>2.0525713862632945E-2</v>
+        <v>2.0460765142843514E-2</v>
       </c>
       <c r="R12" s="2">
-        <v>2.7966562536942543E-2</v>
+        <v>2.798323054501933E-2</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>5.1519304202631965E-3</v>
+        <v>5.3785052731830461E-3</v>
       </c>
       <c r="B13" s="2">
-        <v>2.8855251976566281E-2</v>
+        <v>2.6738923838399504E-2</v>
       </c>
       <c r="C13" s="2">
-        <v>9.9999947211530743E-2</v>
+        <v>9.9999999999977537E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>216401436.90357524</v>
+        <v>216470048.14877984</v>
       </c>
       <c r="E13" s="2">
-        <v>28.426368858582276</v>
+        <v>28.433727230396499</v>
       </c>
       <c r="F13" s="2">
-        <v>54.929167693269896</v>
+        <v>54.906064887553164</v>
       </c>
       <c r="G13" s="2">
-        <v>2.4016579977139205E-4</v>
+        <v>3.2756574456477034E-4</v>
       </c>
       <c r="H13" s="2">
-        <v>2.7256318248896662E-2</v>
+        <v>1.9699840230101226E-2</v>
       </c>
       <c r="I13" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.2218515143462973E-14</v>
       </c>
       <c r="J13" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999999999769631E-3</v>
       </c>
       <c r="K13" s="2">
-        <v>0.99860148353106892</v>
+        <v>0.99860127036337543</v>
       </c>
       <c r="L13" s="2">
-        <v>0.99424611287246834</v>
+        <v>0.99478661481358055</v>
       </c>
       <c r="M13" s="2">
-        <v>0.98838609410607781</v>
+        <v>0.98959205188990085</v>
       </c>
       <c r="N13" s="2">
-        <v>3.7209290563537098E-2</v>
+        <v>3.7212126252853521E-2</v>
       </c>
       <c r="O13" s="2">
-        <v>7.5474156214272448E-2</v>
+        <v>7.184184946502474E-2</v>
       </c>
       <c r="P13" s="2">
-        <v>0.10722764025652617</v>
+        <v>0.1015079732286986</v>
       </c>
       <c r="Q13" s="2">
-        <v>1.9609167295389317E-2</v>
+        <v>1.9609087170804188E-2</v>
       </c>
       <c r="R13" s="2">
-        <v>2.6622320963507355E-2</v>
+        <v>2.6532400155956409E-2</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>3.696359030175931E-3</v>
+        <v>3.7811522215408897E-3</v>
       </c>
       <c r="B14" s="2">
-        <v>2.5118050812207509E-2</v>
+        <v>2.3975951449874546E-2</v>
       </c>
       <c r="C14" s="2">
-        <v>3.1655629434963514E-2</v>
+        <v>3.7648713267753244E-2</v>
       </c>
       <c r="D14" s="2">
-        <v>2495250970.1058059</v>
+        <v>2505929597.0853271</v>
       </c>
       <c r="E14" s="2">
-        <v>33.02064487764649</v>
+        <v>33.023920788383059</v>
       </c>
       <c r="F14" s="2">
-        <v>59.464149160759526</v>
+        <v>59.464307434542782</v>
       </c>
       <c r="G14" s="2">
-        <v>0.73046171235060575</v>
+        <v>0.73367388393967248</v>
       </c>
       <c r="H14" s="2">
-        <v>2.2592137752089961E-2</v>
+        <v>7.8385779505851828E-3</v>
       </c>
       <c r="I14" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999866391353946E-3</v>
       </c>
       <c r="J14" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>4.7372018157425733E-12</v>
       </c>
       <c r="K14" s="2">
-        <v>0.99716396915544014</v>
+        <v>0.99716413840400764</v>
       </c>
       <c r="L14" s="2">
-        <v>0.99306798344342373</v>
+        <v>0.99336359824611264</v>
       </c>
       <c r="M14" s="2">
-        <v>0.99214948395361646</v>
+        <v>0.99192791876802611</v>
       </c>
       <c r="N14" s="2">
-        <v>5.298745640351344E-2</v>
+        <v>5.2985875287971357E-2</v>
       </c>
       <c r="O14" s="2">
-        <v>8.2841392980867429E-2</v>
+        <v>8.1055769297123478E-2</v>
       </c>
       <c r="P14" s="2">
-        <v>8.8159009102415059E-2</v>
+        <v>8.9394409331088304E-2</v>
       </c>
       <c r="Q14" s="2">
-        <v>2.1164592113205351E-2</v>
+        <v>2.1234380756629898E-2</v>
       </c>
       <c r="R14" s="2">
-        <v>2.6562311963215065E-2</v>
+        <v>2.652705700243119E-2</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>5.6207319018958448E-3</v>
+        <v>5.733412868772542E-3</v>
       </c>
       <c r="B15" s="2">
-        <v>4.5167341335324525E-2</v>
+        <v>4.4777155572905403E-2</v>
       </c>
       <c r="C15" s="2">
-        <v>9.1142339946662779E-2</v>
+        <v>8.5142842438287111E-2</v>
       </c>
       <c r="D15" s="2">
-        <v>218581353.42297032</v>
+        <v>218002613.50193721</v>
       </c>
       <c r="E15" s="2">
-        <v>17.965343306105765</v>
+        <v>17.966340175817113</v>
       </c>
       <c r="F15" s="2">
-        <v>65.96941977258993</v>
+        <v>65.908559158253198</v>
       </c>
       <c r="G15" s="2">
-        <v>1.0000040928157862E-8</v>
+        <v>1.0000042249550875E-8</v>
       </c>
       <c r="H15" s="2">
-        <v>6.979874171140172E-3</v>
+        <v>6.2919062710599565E-3</v>
       </c>
       <c r="I15" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.4289203051887389E-11</v>
       </c>
       <c r="J15" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999958653245423E-3</v>
       </c>
       <c r="K15" s="2">
-        <v>0.99870352220968939</v>
+        <v>0.99870449586169496</v>
       </c>
       <c r="L15" s="2">
-        <v>0.98710494737937005</v>
+        <v>0.98769404147713824</v>
       </c>
       <c r="M15" s="2">
-        <v>0.99315159156446964</v>
+        <v>0.99309265476941699</v>
       </c>
       <c r="N15" s="2">
-        <v>3.5826149840688437E-2</v>
+        <v>3.5812694633635289E-2</v>
       </c>
       <c r="O15" s="2">
-        <v>0.11298717668135487</v>
+        <v>0.11037617015295072</v>
       </c>
       <c r="P15" s="2">
-        <v>8.2340296035264757E-2</v>
+        <v>8.2693843654029875E-2</v>
       </c>
       <c r="Q15" s="2">
-        <v>1.9607843137295827E-2</v>
+        <v>1.9607843137297149E-2</v>
       </c>
       <c r="R15" s="2">
-        <v>2.6528605712791618E-2</v>
+        <v>2.6528384440147008E-2</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>5.3062504808824356E-3</v>
+        <v>5.2165143665999902E-3</v>
       </c>
       <c r="B16" s="2">
-        <v>0.61291947765886456</v>
+        <v>0.58116457014490119</v>
       </c>
       <c r="C16" s="2">
-        <v>7.8956042893276665E-2</v>
+        <v>9.8639936921224136E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>1519949810.6435816</v>
+        <v>1520028310.508136</v>
       </c>
       <c r="E16" s="2">
-        <v>42.233803493362387</v>
+        <v>42.233909335383906</v>
       </c>
       <c r="F16" s="2">
-        <v>67.258572902964147</v>
+        <v>67.258477067235617</v>
       </c>
       <c r="G16" s="2">
-        <v>0.6521357459980327</v>
+        <v>0.65224422154978035</v>
       </c>
       <c r="H16" s="2">
-        <v>3.1123639904761689</v>
+        <v>2.9445381858027808</v>
       </c>
       <c r="I16" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.2114734400216535E-4</v>
       </c>
       <c r="J16" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.7466018319122646E-7</v>
       </c>
       <c r="K16" s="2">
-        <v>0.99372489452667079</v>
+        <v>0.99372489864384794</v>
       </c>
       <c r="L16" s="2">
-        <v>0.96469026575064731</v>
+        <v>0.96467753514876009</v>
       </c>
       <c r="M16" s="2">
-        <v>0.9127663741997234</v>
+        <v>0.91329113989406796</v>
       </c>
       <c r="N16" s="2">
-        <v>7.8818490334413085E-2</v>
+        <v>7.8818464477497449E-2</v>
       </c>
       <c r="O16" s="2">
-        <v>0.18696694067898509</v>
+        <v>0.18700064225217924</v>
       </c>
       <c r="P16" s="2">
-        <v>0.29387291393096082</v>
+        <v>0.29298766442441349</v>
       </c>
       <c r="Q16" s="2">
-        <v>2.1256107184652727E-2</v>
+        <v>2.1276009206649304E-2</v>
       </c>
       <c r="R16" s="2">
-        <v>2.7340610508093041E-2</v>
+        <v>2.7041107086627207E-2</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>8.3183993151910388E-3</v>
+        <v>8.6066060331552955E-3</v>
       </c>
       <c r="B17" s="2">
-        <v>0.16228696157400924</v>
+        <v>0.16008235012557337</v>
       </c>
       <c r="C17" s="2">
-        <v>9.6384269631279745E-2</v>
+        <v>9.9339087276265128E-2</v>
       </c>
       <c r="D17" s="2">
-        <v>57116386.347033344</v>
+        <v>57131236.229517505</v>
       </c>
       <c r="E17" s="2">
-        <v>32.73420902555101</v>
+        <v>32.736381824141198</v>
       </c>
       <c r="F17" s="2">
-        <v>55.193140966553017</v>
+        <v>55.183442677006219</v>
       </c>
       <c r="G17" s="2">
-        <v>1.0000042766914775E-8</v>
+        <v>9.3204360810517093E-8</v>
       </c>
       <c r="H17" s="2">
-        <v>4.8023719675805085E-2</v>
+        <v>4.6292385710475975E-2</v>
       </c>
       <c r="I17" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>5.5963149063981782E-13</v>
       </c>
       <c r="J17" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9042611482077596E-3</v>
       </c>
       <c r="K17" s="2">
-        <v>0.996161052117575</v>
+        <v>0.99616058103576866</v>
       </c>
       <c r="L17" s="2">
-        <v>0.98099156214913619</v>
+        <v>0.98170981704693761</v>
       </c>
       <c r="M17" s="2">
-        <v>0.99514615842985477</v>
+        <v>0.9951918161648281</v>
       </c>
       <c r="N17" s="2">
-        <v>6.164866911459483E-2</v>
+        <v>6.1652451488882459E-2</v>
       </c>
       <c r="O17" s="2">
-        <v>0.13718000390856966</v>
+        <v>0.13456329783240231</v>
       </c>
       <c r="P17" s="2">
-        <v>6.9320293958146165E-2</v>
+        <v>6.8993492423707725E-2</v>
       </c>
       <c r="Q17" s="2">
-        <v>1.960784313729767E-2</v>
+        <v>1.9607851016459839E-2</v>
       </c>
       <c r="R17" s="2">
-        <v>2.6573144969216398E-2</v>
+        <v>2.6583396901367802E-2</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>2.2227626629960973E-2</v>
+        <v>2.3825085307432405E-2</v>
       </c>
       <c r="B18" s="2">
-        <v>0.4455143893608759</v>
+        <v>0.4868769103206117</v>
       </c>
       <c r="C18" s="2">
-        <v>9.9999928835932686E-2</v>
+        <v>9.9999899886540525E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>1831654156.4629984</v>
+        <v>1719077230.4604545</v>
       </c>
       <c r="E18" s="2">
-        <v>13.76238139991213</v>
+        <v>13.702998564284247</v>
       </c>
       <c r="F18" s="2">
-        <v>72.559335178158378</v>
+        <v>72.555247982805568</v>
       </c>
       <c r="G18" s="2">
-        <v>0.55600349362331136</v>
+        <v>0.51501016025399993</v>
       </c>
       <c r="H18" s="2">
-        <v>0.28033173702274161</v>
+        <v>0.31446067020291762</v>
       </c>
       <c r="I18" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>2.6497694029687907E-5</v>
       </c>
       <c r="J18" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.8250572295691101E-4</v>
       </c>
       <c r="K18" s="2">
-        <v>0.99527508878899518</v>
+        <v>0.99526522827522435</v>
       </c>
       <c r="L18" s="2">
-        <v>0.96683225774264592</v>
+        <v>0.96728956190212578</v>
       </c>
       <c r="M18" s="2">
-        <v>0.99058286386747396</v>
+        <v>0.99004082044259878</v>
       </c>
       <c r="N18" s="2">
-        <v>6.8393436080480721E-2</v>
+        <v>6.8464764715347251E-2</v>
       </c>
       <c r="O18" s="2">
-        <v>0.18120724277682862</v>
+        <v>0.17995369881415477</v>
       </c>
       <c r="P18" s="2">
-        <v>9.6555500988813395E-2</v>
+        <v>9.9295456904267068E-2</v>
       </c>
       <c r="Q18" s="2">
-        <v>2.0775048602772368E-2</v>
+        <v>2.1120254939138508E-2</v>
       </c>
       <c r="R18" s="2">
-        <v>2.6843185302714068E-2</v>
+        <v>2.677546499569956E-2</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -9655,223 +8781,223 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="B19" s="2">
-        <v>8.9660258899521852E-2</v>
+        <v>8.9660203498313579E-2</v>
       </c>
       <c r="C19" s="2">
-        <v>2.6315789473706427E-2</v>
+        <v>2.6315789473706417E-2</v>
       </c>
       <c r="D19" s="2">
-        <v>50540598.95140136</v>
+        <v>50540648.358700573</v>
       </c>
       <c r="E19" s="2">
-        <v>25.913986129981062</v>
+        <v>25.91398305976729</v>
       </c>
       <c r="F19" s="2">
-        <v>62.398220587373139</v>
+        <v>62.398234066853576</v>
       </c>
       <c r="G19" s="2">
-        <v>0.60867035151505011</v>
+        <v>0.60832421319523755</v>
       </c>
       <c r="H19" s="2">
-        <v>2.7326222578025389E-2</v>
+        <v>2.7316030758319766E-2</v>
       </c>
       <c r="I19" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.2229931290132734E-14</v>
       </c>
       <c r="J19" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.220511957324058E-14</v>
       </c>
       <c r="K19" s="2">
-        <v>0.98245584466323166</v>
+        <v>0.98245588834946462</v>
       </c>
       <c r="L19" s="2">
-        <v>0.9313169311113072</v>
+        <v>0.93131688102757759</v>
       </c>
       <c r="M19" s="2">
-        <v>0.93502010667144464</v>
+        <v>0.93501999229245869</v>
       </c>
       <c r="N19" s="2">
-        <v>0.13179041612879369</v>
+        <v>0.13179025204479272</v>
       </c>
       <c r="O19" s="2">
-        <v>0.26076088318573759</v>
+        <v>0.26076097825920619</v>
       </c>
       <c r="P19" s="2">
-        <v>0.25363378007526877</v>
+        <v>0.25363400330094915</v>
       </c>
       <c r="Q19" s="2">
-        <v>2.0875574745586396E-2</v>
+        <v>2.1222426286284703E-2</v>
       </c>
       <c r="R19" s="2">
-        <v>2.6558097844496347E-2</v>
+        <v>2.6568225637508797E-2</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>1.0575516431258088E-2</v>
+        <v>1.0760566128758033E-2</v>
       </c>
       <c r="B20" s="2">
-        <v>0.11351920357952909</v>
+        <v>0.10810136923207164</v>
       </c>
       <c r="C20" s="2">
-        <v>9.9996154785638877E-2</v>
+        <v>9.9999999990512817E-2</v>
       </c>
       <c r="D20" s="2">
-        <v>1442195150.8003712</v>
+        <v>1442195496.1246281</v>
       </c>
       <c r="E20" s="2">
-        <v>21.073200082662254</v>
+        <v>21.071901191010653</v>
       </c>
       <c r="F20" s="2">
-        <v>66.226022643653195</v>
+        <v>66.224947910183658</v>
       </c>
       <c r="G20" s="2">
-        <v>0.64145927673503045</v>
+        <v>0.64179913127875132</v>
       </c>
       <c r="H20" s="2">
-        <v>0.12935499209510501</v>
+        <v>0.1195542193137312</v>
       </c>
       <c r="I20" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>1.001442476453742E-9</v>
       </c>
       <c r="J20" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9992167257435018E-3</v>
       </c>
       <c r="K20" s="2">
-        <v>0.99429033921516119</v>
+        <v>0.99428979846547727</v>
       </c>
       <c r="L20" s="2">
-        <v>0.99110919057621594</v>
+        <v>0.99141974525984633</v>
       </c>
       <c r="M20" s="2">
-        <v>0.98947858595712912</v>
+        <v>0.99018690753118732</v>
       </c>
       <c r="N20" s="2">
-        <v>7.5183536608691551E-2</v>
+        <v>7.5187096759866429E-2</v>
       </c>
       <c r="O20" s="2">
-        <v>9.3818448769665122E-2</v>
+        <v>9.2165352452817859E-2</v>
       </c>
       <c r="P20" s="2">
-        <v>0.10205978592198878</v>
+        <v>9.8564504483736548E-2</v>
       </c>
       <c r="Q20" s="2">
-        <v>2.0902529677286813E-2</v>
+        <v>2.0784713283118691E-2</v>
       </c>
       <c r="R20" s="2">
-        <v>2.6623766806585347E-2</v>
+        <v>2.6593421852223683E-2</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>7.5658256135292361E-3</v>
+        <v>7.6944322146647853E-3</v>
       </c>
       <c r="B21" s="2">
-        <v>0.19069628558421536</v>
+        <v>0.18642571809378297</v>
       </c>
       <c r="C21" s="2">
-        <v>9.9999643553698392E-2</v>
+        <v>9.9999999999977593E-2</v>
       </c>
       <c r="D21" s="2">
-        <v>2066751785.564697</v>
+        <v>2066749147.1669409</v>
       </c>
       <c r="E21" s="2">
-        <v>15.152701909467437</v>
+        <v>15.152081001230075</v>
       </c>
       <c r="F21" s="2">
-        <v>69.229945500553924</v>
+        <v>69.229555840732246</v>
       </c>
       <c r="G21" s="2">
-        <v>0.62049862141063672</v>
+        <v>0.62044499916990414</v>
       </c>
       <c r="H21" s="2">
-        <v>0.14987985901719575</v>
+        <v>0.1447969226843194</v>
       </c>
       <c r="I21" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>3.2204898710353411E-14</v>
       </c>
       <c r="J21" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>9.9999993926586754E-3</v>
       </c>
       <c r="K21" s="2">
-        <v>0.98943808559420809</v>
+        <v>0.9894380131515057</v>
       </c>
       <c r="L21" s="2">
-        <v>0.98032463795454661</v>
+        <v>0.98056065158178418</v>
       </c>
       <c r="M21" s="2">
-        <v>0.98149682656043036</v>
+        <v>0.98156151094688882</v>
       </c>
       <c r="N21" s="2">
-        <v>0.10225602799705244</v>
+        <v>0.10225637867639044</v>
       </c>
       <c r="O21" s="2">
-        <v>0.13956578529495983</v>
+        <v>0.13872618690800109</v>
       </c>
       <c r="P21" s="2">
-        <v>0.13534452964628443</v>
+        <v>0.1351077501943542</v>
       </c>
       <c r="Q21" s="2">
-        <v>2.0785424222386318E-2</v>
+        <v>2.0934129971447942E-2</v>
       </c>
       <c r="R21" s="2">
-        <v>2.6748827653118732E-2</v>
+        <v>2.6807441557686947E-2</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>6.7368678399530695E-3</v>
+        <v>6.7424239870017616E-3</v>
       </c>
       <c r="B22" s="2">
-        <v>0.22275044511979611</v>
+        <v>0.22304305297682125</v>
       </c>
       <c r="C22" s="2">
-        <v>9.9999578942145145E-2</v>
+        <v>9.9998601617137084E-2</v>
       </c>
       <c r="D22" s="2">
-        <v>1070399356.6897655</v>
+        <v>1070399379.5138259</v>
       </c>
       <c r="E22" s="2">
-        <v>15.623724171703495</v>
+        <v>15.623216818777985</v>
       </c>
       <c r="F22" s="2">
-        <v>75.123508421097199</v>
+        <v>75.124014324750945</v>
       </c>
       <c r="G22" s="2">
-        <v>0.54387352989611515</v>
+        <v>0.54387845927072231</v>
       </c>
       <c r="H22" s="2">
-        <v>0.18231571085823212</v>
+        <v>0.18267324308497107</v>
       </c>
       <c r="I22" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>7.888151888538791E-7</v>
       </c>
       <c r="J22" s="2">
-        <v>5.0000000000050004E-3</v>
+        <v>4.182288630781361E-7</v>
       </c>
       <c r="K22" s="2">
-        <v>0.99162805397818088</v>
+        <v>0.99162805449586033</v>
       </c>
       <c r="L22" s="2">
-        <v>0.93841327370491479</v>
+        <v>0.93842985926322897</v>
       </c>
       <c r="M22" s="2">
-        <v>0.99214611935874997</v>
+        <v>0.99211803884111582</v>
       </c>
       <c r="N22" s="2">
-        <v>9.1039697723580698E-2</v>
+        <v>9.1039694908859492E-2</v>
       </c>
       <c r="O22" s="2">
-        <v>0.24692277949216099</v>
+        <v>0.24688952859407243</v>
       </c>
       <c r="P22" s="2">
-        <v>8.8177898788968478E-2</v>
+        <v>8.8335392382076133E-2</v>
       </c>
       <c r="Q22" s="2">
-        <v>2.0587448456778363E-2</v>
+        <v>2.0575461872008087E-2</v>
       </c>
       <c r="R22" s="2">
-        <v>2.6743255506806514E-2</v>
+        <v>2.6748083524552567E-2</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -9927,7 +9053,7 @@
       </c>
       <c r="V23" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="W23" t="str">
         <f t="shared" si="0"/>
@@ -9948,27 +9074,27 @@
       </c>
       <c r="B24" s="2">
         <f>AVERAGE(A$1:A$3)</f>
-        <v>2.3164158690311869E-3</v>
+        <v>2.3173268963984188E-3</v>
       </c>
       <c r="C24" s="2">
         <f>AVERAGE(A$4:A$6)</f>
-        <v>6.3841099779699843E-3</v>
+        <v>6.5132119631182801E-3</v>
       </c>
       <c r="D24" s="2">
         <f>AVERAGE(A$7:A$12,A$17:A$19)</f>
-        <v>2.7259684965693379E-2</v>
+        <v>2.7535106283079838E-2</v>
       </c>
       <c r="E24" s="2">
         <f>AVERAGE(A$13:A$16)</f>
-        <v>4.9438179583043522E-3</v>
+        <v>5.0273961825241173E-3</v>
       </c>
       <c r="F24" s="2">
         <f>A$20</f>
-        <v>1.0575516431258088E-2</v>
+        <v>1.0760566128758033E-2</v>
       </c>
       <c r="G24" s="2">
         <f>AVERAGE(A$21:A$22)</f>
-        <v>7.1513467267411528E-3</v>
+        <v>7.218428100833273E-3</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" ref="N24:N44" si="2">_xlfn.IFS(ABS(A2-T$5)&lt;=0.01*T$5,"Lower",ABS(A2-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
@@ -9980,7 +9106,7 @@
       </c>
       <c r="P24" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="0"/>
@@ -9996,7 +9122,7 @@
       </c>
       <c r="T24" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U24" t="str">
         <f t="shared" si="0"/>
@@ -10022,24 +9148,24 @@
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <f>STDEV(A$1:A$3)/SQRT(COUNT(A$1:A$3))</f>
-        <v>1.4394371902156326E-4</v>
+        <v>1.4110540454517E-4</v>
       </c>
       <c r="C25" s="2">
         <f>STDEV(A$4:A$6)/SQRT(COUNT(A$4:A$6))</f>
-        <v>1.1454985630101012E-3</v>
+        <v>1.1938388220454957E-3</v>
       </c>
       <c r="D25" s="2">
         <f>STDEV(A$7:A$12,A$17:A$19)/SQRT(COUNT(A$7:A$12,A$17:A$19))</f>
-        <v>1.0252324897493665E-2</v>
+        <v>1.0219978638120604E-2</v>
       </c>
       <c r="E25" s="2">
         <f>STDEV(A$13:A$16)/SQRT(COUNT(A$13:A$16))</f>
-        <v>4.2710599724978308E-4</v>
+        <v>4.2920729768569356E-4</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
         <f>STDEV(A$21:A$22)/SQRT(COUNT(A$21:A$22))</f>
-        <v>4.1447888678808326E-4</v>
+        <v>4.7600411383151179E-4</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="2"/>
@@ -10129,7 +9255,7 @@
       </c>
       <c r="W26" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="1"/>
@@ -10137,7 +9263,7 @@
       </c>
       <c r="AE26" t="str">
         <f t="shared" si="1"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -10169,7 +9295,7 @@
       </c>
       <c r="P27" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="0"/>
@@ -10214,27 +9340,27 @@
       </c>
       <c r="C28" s="2">
         <f>AVERAGE(B$1:B$3)</f>
-        <v>9.1562026481064915E-2</v>
+        <v>9.2535545750464687E-2</v>
       </c>
       <c r="D28" s="2">
         <f>AVERAGE(B$4:B$6)</f>
-        <v>0.35224348703388203</v>
+        <v>0.3541415185008206</v>
       </c>
       <c r="E28" s="2">
         <f>AVERAGE(B$7:B$12,B$17:B$19)</f>
-        <v>0.74774420072208381</v>
+        <v>0.75444268232926348</v>
       </c>
       <c r="F28" s="2">
         <f>AVERAGE(B$13:B$16)</f>
-        <v>0.17801503044574071</v>
+        <v>0.16916415025152015</v>
       </c>
       <c r="G28" s="2">
         <f>B$20</f>
-        <v>0.11351920357952909</v>
+        <v>0.10810136923207164</v>
       </c>
       <c r="H28" s="2">
         <f>AVERAGE(B$21:B$22)</f>
-        <v>0.20672336535200575</v>
+        <v>0.2047343855353021</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="2"/>
@@ -10262,7 +9388,7 @@
       </c>
       <c r="T28" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U28" t="str">
         <f t="shared" si="0"/>
@@ -10274,7 +9400,7 @@
       </c>
       <c r="W28" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="1"/>
@@ -10288,24 +9414,24 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
-        <v>1.0119091447892565E-2</v>
+        <v>1.2057455739979463E-2</v>
       </c>
       <c r="D29" s="2">
         <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
-        <v>5.4093217675224937E-2</v>
+        <v>5.7309495294150879E-2</v>
       </c>
       <c r="E29" s="2">
         <f>STDEV(B$7:B$12,B$17:B$19)/SQRT(COUNT(B$7:B$12,B$17:B$19))</f>
-        <v>0.39819613118576136</v>
+        <v>0.39928208436858398</v>
       </c>
       <c r="F29" s="2">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
-        <v>0.14503347676822781</v>
+        <v>0.13741088889033834</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
         <f>STDEV(B$21:B$22)/SQRT(COUNT(B$21:B$22))</f>
-        <v>1.6027079767790373E-2</v>
+        <v>1.8308667441519141E-2</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="2"/>
@@ -10341,7 +9467,7 @@
       </c>
       <c r="V29" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="0"/>
@@ -10399,7 +9525,7 @@
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="1"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="AE30" t="str">
         <f t="shared" si="1"/>
@@ -10480,27 +9606,27 @@
       </c>
       <c r="D32" s="2">
         <f>AVERAGE(C$1:C$3)</f>
-        <v>7.5338792243522842E-2</v>
+        <v>7.384890314233869E-2</v>
       </c>
       <c r="E32" s="2">
         <f>AVERAGE(C$4:C$6)</f>
-        <v>5.0878096231398669E-2</v>
+        <v>5.0263555960985945E-2</v>
       </c>
       <c r="F32" s="2">
         <f>AVERAGE(C$7:C$12,C$17:C$19)</f>
-        <v>5.9605294490649968E-2</v>
+        <v>6.3109847044927683E-2</v>
       </c>
       <c r="G32" s="2">
         <f>AVERAGE(C$13:C$16)</f>
-        <v>7.5438489871608422E-2</v>
+        <v>8.0357873156810505E-2</v>
       </c>
       <c r="H32" s="2">
         <f>C$20</f>
-        <v>9.9996154785638877E-2</v>
+        <v>9.9999999990512817E-2</v>
       </c>
       <c r="I32" s="2">
         <f>AVERAGE(C$21:C$22)</f>
-        <v>9.9999611247921769E-2</v>
+        <v>9.9999300808557345E-2</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="2"/>
@@ -10548,30 +9674,30 @@
       </c>
       <c r="AE32" t="str">
         <f t="shared" si="1"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
     </row>
     <row r="33" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
-        <v>2.4510193064883369E-2</v>
+        <v>2.3803754511435734E-2</v>
       </c>
       <c r="E33" s="2">
         <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
-        <v>2.4560951831086825E-2</v>
+        <v>2.3947765296666392E-2</v>
       </c>
       <c r="F33" s="2">
         <f>STDEV(C$7:C$12,C$17:C$19)/SQRT(COUNT(C$7:C$12,C$17:C$19))</f>
-        <v>1.117040559412727E-2</v>
+        <v>1.0466686942143609E-2</v>
       </c>
       <c r="G33" s="2">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
-        <v>1.5218377435181186E-2</v>
+        <v>1.4625933793160245E-2</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2">
         <f>STDEV(C$21:C$22)/SQRT(COUNT(C$21:C$22))</f>
-        <v>3.2305776623275939E-8</v>
+        <v>6.9919142025448567E-7</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="2"/>
@@ -10729,7 +9855,7 @@
       </c>
       <c r="W35" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD35" t="str">
         <f t="shared" si="1"/>
@@ -10746,27 +9872,27 @@
       </c>
       <c r="E36" s="2">
         <f>AVERAGE(D$1:D$3)</f>
-        <v>632012098.83339036</v>
+        <v>632008997.85957575</v>
       </c>
       <c r="F36" s="2">
         <f>AVERAGE(D$4:D$6)</f>
-        <v>429395903.73384517</v>
+        <v>429383170.13780922</v>
       </c>
       <c r="G36" s="2">
         <f>AVERAGE(D$7:D$12,D$17:D$19)</f>
-        <v>669616800.65452504</v>
+        <v>657231049.83675289</v>
       </c>
       <c r="H36" s="2">
         <f>AVERAGE(D$13:D$16)</f>
-        <v>1112545892.7689834</v>
+        <v>1115107642.3110452</v>
       </c>
       <c r="I36" s="2">
         <f>D$20</f>
-        <v>1442195150.8003712</v>
+        <v>1442195496.1246281</v>
       </c>
       <c r="J36" s="2">
         <f>AVERAGE(D$21:D$22)</f>
-        <v>1568575571.1272311</v>
+        <v>1568574263.3403835</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="2"/>
@@ -10802,7 +9928,7 @@
       </c>
       <c r="V36" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="W36" t="str">
         <f t="shared" si="0"/>
@@ -10820,24 +9946,24 @@
     <row r="37" spans="4:31" x14ac:dyDescent="0.25">
       <c r="E37" s="2">
         <f>STDEV(D$1:D$3)/SQRT(COUNT(D$1:D$3))</f>
-        <v>304771761.86323607</v>
+        <v>304779407.73467177</v>
       </c>
       <c r="F37" s="2">
         <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
-        <v>337005855.24468315</v>
+        <v>337009161.21699256</v>
       </c>
       <c r="G37" s="2">
         <f>STDEV(D$7:D$12,D$17:D$19)/SQRT(COUNT(D$7:D$12,D$17:D$19))</f>
-        <v>225598503.03394902</v>
+        <v>217752834.47134462</v>
       </c>
       <c r="H37" s="2">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
-        <v>553782355.45647335</v>
+        <v>556079536.85988617</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2">
         <f>STDEV(D$21:D$22)/SQRT(COUNT(D$21:D$22))</f>
-        <v>498176214.43746614</v>
+        <v>498174883.8265568</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="2"/>
@@ -10877,7 +10003,7 @@
       </c>
       <c r="W37" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD37" t="str">
         <f t="shared" si="1"/>
@@ -10967,7 +10093,7 @@
       </c>
       <c r="P39" t="str">
         <f t="shared" ref="P39:P44" si="4">_xlfn.IFS(ABS(C17-V$5)&lt;=0.01*V$5,"Lower",ABS(C17-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ref="Q39:Q44" si="5">_xlfn.IFS(ABS(D17-W$5)&lt;=0.01*W$5,"Lower",ABS(D17-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
@@ -10983,7 +10109,7 @@
       </c>
       <c r="T39" t="str">
         <f t="shared" ref="T39:T44" si="8">_xlfn.IFS(ABS(G17-Z$5)&lt;=0.01*Z$5,"Lower",ABS(G17-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U39" t="str">
         <f t="shared" ref="U39:U44" si="9">_xlfn.IFS(ABS(H17-AA$5)&lt;=0.01*AA$5,"Lower",ABS(H17-AA$6)&lt;=0.01*AA$6,"Upper",TRUE,"Ok")</f>
@@ -10995,7 +10121,7 @@
       </c>
       <c r="W39" t="str">
         <f t="shared" ref="W39:W44" si="11">_xlfn.IFS(ABS(J17-AC$5)&lt;=0.01*AC$5,"Lower",ABS(J17-AC$6)&lt;=0.01*AC$6,"Upper",TRUE,"Ok")</f>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD39" t="str">
         <f t="shared" si="1"/>
@@ -11012,27 +10138,27 @@
       </c>
       <c r="F40" s="2">
         <f>AVERAGE(E$1:E$3)</f>
-        <v>20.568721823519486</v>
+        <v>20.569031590712743</v>
       </c>
       <c r="G40" s="2">
         <f>AVERAGE(E$4:E$6)</f>
-        <v>22.075998539826269</v>
+        <v>22.076323769486507</v>
       </c>
       <c r="H40" s="2">
         <f>AVERAGE(E$7:E$12,E$17:E$19)</f>
-        <v>27.055312017837505</v>
+        <v>27.049486754336399</v>
       </c>
       <c r="I40" s="2">
         <f>AVERAGE(E$13:E$16)</f>
-        <v>30.41154013392423</v>
+        <v>30.414474382495143</v>
       </c>
       <c r="J40" s="2">
         <f>E$20</f>
-        <v>21.073200082662254</v>
+        <v>21.071901191010653</v>
       </c>
       <c r="K40" s="2">
         <f>AVERAGE(E$21:E$22)</f>
-        <v>15.388213040585466</v>
+        <v>15.38764891000403</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="2"/>
@@ -11076,34 +10202,34 @@
       </c>
       <c r="AD40" t="str">
         <f t="shared" si="1"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="AE40" t="str">
         <f t="shared" si="1"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
     </row>
     <row r="41" spans="4:31" x14ac:dyDescent="0.25">
       <c r="F41" s="2">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
-        <v>1.6354276925167162</v>
+        <v>1.6353604324085522</v>
       </c>
       <c r="G41" s="2">
         <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
-        <v>5.4275970119096479</v>
+        <v>5.4277614734308957</v>
       </c>
       <c r="H41" s="2">
         <f>STDEV(E$7:E$12,E$17:E$19)/SQRT(COUNT(E$7:E$12,E$17:E$19))</f>
-        <v>3.3651259367796573</v>
+        <v>3.3683323128668317</v>
       </c>
       <c r="I41" s="2">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
-        <v>5.0449814913177899</v>
+        <v>5.0446973617418731</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2">
         <f>STDEV(E$21:E$22)/SQRT(COUNT(E$21:E$22))</f>
-        <v>0.23551113111802913</v>
+        <v>0.23556790877395525</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="2"/>
@@ -11147,7 +10273,7 @@
       </c>
       <c r="AD41" t="str">
         <f t="shared" si="1"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="AE41" t="str">
         <f t="shared" si="1"/>
@@ -11193,7 +10319,7 @@
       </c>
       <c r="W42" t="str">
         <f t="shared" si="11"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD42" t="str">
         <f t="shared" si="1"/>
@@ -11261,7 +10387,7 @@
       </c>
       <c r="W43" t="str">
         <f t="shared" si="11"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="AD43" t="str">
         <f t="shared" si="1"/>
@@ -11269,7 +10395,7 @@
       </c>
       <c r="AE43" t="str">
         <f t="shared" si="1"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="44" spans="4:31" x14ac:dyDescent="0.25">
@@ -11278,27 +10404,27 @@
       </c>
       <c r="G44" s="2">
         <f>AVERAGE(F$1:F$3)</f>
-        <v>62.934262420288405</v>
+        <v>62.929200798475335</v>
       </c>
       <c r="H44" s="2">
         <f>AVERAGE(F$4:F$6)</f>
-        <v>61.05613251932985</v>
+        <v>61.049871234843614</v>
       </c>
       <c r="I44" s="2">
         <f>AVERAGE(F$7:F$12,F$17:F$19)</f>
-        <v>62.567355798911727</v>
+        <v>62.565940988884485</v>
       </c>
       <c r="J44" s="2">
         <f>AVERAGE(F$13:F$16)</f>
-        <v>61.905327382395875</v>
+        <v>61.88435213689619</v>
       </c>
       <c r="K44" s="2">
         <f>F$20</f>
-        <v>66.226022643653195</v>
+        <v>66.224947910183658</v>
       </c>
       <c r="L44" s="2">
         <f>AVERAGE(F$21:F$22)</f>
-        <v>72.176726960825562</v>
+        <v>72.176785082741588</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="2"/>
@@ -11352,24 +10478,24 @@
     <row r="45" spans="4:31" x14ac:dyDescent="0.25">
       <c r="G45" s="2">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
-        <v>3.0896746143542604</v>
+        <v>3.0934409159415974</v>
       </c>
       <c r="H45" s="2">
         <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
-        <v>4.8859616724569772</v>
+        <v>4.888968988250177</v>
       </c>
       <c r="I45" s="2">
         <f>STDEV(F$7:F$12,F$17:F$19)/SQRT(COUNT(F$7:F$12,F$17:F$19))</f>
-        <v>3.8235767414533695</v>
+        <v>3.824336547084958</v>
       </c>
       <c r="J45" s="2">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
-        <v>2.8838666126905528</v>
+        <v>2.8813852312930881</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2">
         <f>STDEV(F$21:F$22)/SQRT(COUNT(F$21:F$22))</f>
-        <v>2.9467814602716373</v>
+        <v>2.9472292420093491</v>
       </c>
       <c r="N45" t="s">
         <v>6</v>
@@ -11452,50 +10578,50 @@
       </c>
       <c r="H48" s="2">
         <f>AVERAGE(G$1:G$3)</f>
-        <v>0.43027206758401876</v>
+        <v>0.43030529517923882</v>
       </c>
       <c r="I48" s="2">
         <f>AVERAGE(G$4:G$6)</f>
-        <v>0.19506970397075354</v>
+        <v>0.19506446675691699</v>
       </c>
       <c r="J48" s="2">
         <f>AVERAGE(G$7:G$12,G$17:G$19)</f>
-        <v>0.42067939442780816</v>
+        <v>0.41603336191621143</v>
       </c>
       <c r="K48" s="2">
         <f>AVERAGE(G$13:G$16)</f>
-        <v>0.34570940853711268</v>
+        <v>0.34656142030851494</v>
       </c>
       <c r="L48" s="2">
         <f>G$20</f>
-        <v>0.64145927673503045</v>
+        <v>0.64179913127875132</v>
       </c>
       <c r="M48" s="2">
         <f>AVERAGE(G$21:G$22)</f>
-        <v>0.58218607565337588</v>
+        <v>0.58216172922031317</v>
       </c>
     </row>
     <row r="49" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H49" s="2">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
-        <v>0.21659054729123339</v>
+        <v>0.21660481975386786</v>
       </c>
       <c r="I49" s="2">
         <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
-        <v>0.19506969397072565</v>
+        <v>0.19506444923262076</v>
       </c>
       <c r="J49" s="2">
         <f>STDEV(G$7:G$12,G$17:G$19)/SQRT(COUNT(G$7:G$12,G$17:G$19))</f>
-        <v>0.10282395991032552</v>
+        <v>0.10216020479600753</v>
       </c>
       <c r="K49" s="2">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
-        <v>0.20016564421620908</v>
+        <v>0.20068232101892192</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2">
         <f>STDEV(G$21:G$22)/SQRT(COUNT(G$21:G$22))</f>
-        <v>3.8312545757260785E-2</v>
+        <v>3.8283269949590908E-2</v>
       </c>
     </row>
     <row r="51" spans="8:26" x14ac:dyDescent="0.25">
@@ -11524,50 +10650,50 @@
       </c>
       <c r="I52" s="2">
         <f>AVERAGE(H$1:H$3)</f>
-        <v>3.8181824203370934E-2</v>
+        <v>3.6340015217690251E-2</v>
       </c>
       <c r="J52" s="2">
         <f>AVERAGE(H$4:H$6)</f>
-        <v>0.20297707272718515</v>
+        <v>0.20403788869996353</v>
       </c>
       <c r="K52" s="2">
         <f>AVERAGE(H$7:H$12,H$17:H$19)</f>
-        <v>1.6671523445758363</v>
+        <v>1.6742312906554444</v>
       </c>
       <c r="L52" s="2">
         <f>AVERAGE(H$13:H$16)</f>
-        <v>0.79229808016207393</v>
+        <v>0.7445921275636318</v>
       </c>
       <c r="M52" s="2">
         <f>H$20</f>
-        <v>0.12935499209510501</v>
+        <v>0.1195542193137312</v>
       </c>
       <c r="N52" s="2">
         <f>AVERAGE(H$21:H$22)</f>
-        <v>0.16609778493771393</v>
+        <v>0.16373508288464522</v>
       </c>
     </row>
     <row r="53" spans="8:26" x14ac:dyDescent="0.25">
       <c r="I53" s="2">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
-        <v>1.6355880294056404E-2</v>
+        <v>1.6672231507992838E-2</v>
       </c>
       <c r="J53" s="2">
         <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
-        <v>4.5272571974658983E-2</v>
+        <v>4.6989865419873371E-2</v>
       </c>
       <c r="K53" s="2">
         <f>STDEV(H$7:H$12,H$17:H$19)/SQRT(COUNT(H$7:H$12,H$17:H$19))</f>
-        <v>1.1308271732124933</v>
+        <v>1.1308765015832429</v>
       </c>
       <c r="L53" s="2">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
-        <v>0.77336745514421368</v>
+        <v>0.7333214675380374</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2">
         <f>STDEV(H$21:H$22)/SQRT(COUNT(H$21:H$22))</f>
-        <v>1.6217925920518184E-2</v>
+        <v>1.8938160200325939E-2</v>
       </c>
     </row>
     <row r="55" spans="8:26" x14ac:dyDescent="0.25">
@@ -11596,50 +10722,50 @@
       </c>
       <c r="J56" s="2">
         <f>AVERAGE(I$1:I$3)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>3.3334323368655015E-3</v>
       </c>
       <c r="K56" s="2">
         <f>AVERAGE(I$4:I$6)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>3.547600000994643E-4</v>
       </c>
       <c r="L56" s="2">
         <f>AVERAGE(I$7:I$12,I$17:I$19)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>2.3075847901287152E-3</v>
       </c>
       <c r="M56" s="2">
         <f>AVERAGE(I$13:I$16)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>2.5302835043647456E-3</v>
       </c>
       <c r="N56" s="2">
         <f>I$20</f>
-        <v>5.0000000000050004E-3</v>
+        <v>1.001442476453742E-9</v>
       </c>
       <c r="O56" s="2">
         <f>AVERAGE(I$21:I$22)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>3.9440761052938893E-7</v>
       </c>
     </row>
     <row r="57" spans="8:26" x14ac:dyDescent="0.25">
       <c r="J57" s="2">
         <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
-        <v>0</v>
+        <v>3.3332838326588514E-3</v>
       </c>
       <c r="K57" s="2">
         <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
-        <v>0</v>
+        <v>3.5468109480131071E-4</v>
       </c>
       <c r="L57" s="2">
         <f>STDEV(I$7:I$12,I$17:I$19)/SQRT(COUNT(I$7:I$12,I$17:I$19))</f>
-        <v>0</v>
+        <v>1.1718468534149583E-3</v>
       </c>
       <c r="M57" s="2">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
-        <v>0</v>
+        <v>2.4900647751280795E-3</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2">
         <f>STDEV(I$21:I$22)/SQRT(COUNT(I$21:I$22))</f>
-        <v>0</v>
+        <v>3.9440757832449011E-7</v>
       </c>
     </row>
     <row r="59" spans="8:26" x14ac:dyDescent="0.25">
@@ -11668,50 +10794,50 @@
       </c>
       <c r="K60" s="2">
         <f>AVERAGE(J$1:J$3)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>3.2650559954686166E-3</v>
       </c>
       <c r="L60" s="2">
         <f>AVERAGE(J$4:J$6)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>6.7002828792823597E-3</v>
       </c>
       <c r="M60" s="2">
         <f>AVERAGE(J$7:J$12,J$17:J$19)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>2.3435920833815606E-3</v>
       </c>
       <c r="N60" s="2">
         <f>AVERAGE(J$13:J$16)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>5.0000426325554747E-3</v>
       </c>
       <c r="O60" s="2">
         <f>J$20</f>
-        <v>5.0000000000050004E-3</v>
+        <v>9.9992167257435018E-3</v>
       </c>
       <c r="P60" s="2">
         <f>AVERAGE(J$21:J$22)</f>
-        <v>5.0000000000050004E-3</v>
+        <v>5.0002088107608767E-3</v>
       </c>
     </row>
     <row r="61" spans="8:26" x14ac:dyDescent="0.25">
       <c r="K61" s="2">
         <f>STDEV(J$1:J$3)/SQRT(COUNT(J$1:J$3))</f>
-        <v>0</v>
+        <v>3.2650525106723968E-3</v>
       </c>
       <c r="L61" s="2">
         <f>STDEV(J$4:J$6)/SQRT(COUNT(J$4:J$6))</f>
-        <v>0</v>
+        <v>3.299717120689041E-3</v>
       </c>
       <c r="M61" s="2">
         <f>STDEV(J$7:J$12,J$17:J$19)/SQRT(COUNT(J$7:J$12,J$17:J$19))</f>
-        <v>0</v>
+        <v>1.4092513298116012E-3</v>
       </c>
       <c r="N61" s="2">
         <f>STDEV(J$13:J$16)/SQRT(COUNT(J$13:J$16))</f>
-        <v>0</v>
+        <v>2.8867255386663773E-3</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2">
         <f>STDEV(J$21:J$22)/SQRT(COUNT(J$21:J$22))</f>
-        <v>0</v>
+        <v>4.9997905818977978E-3</v>
       </c>
     </row>
     <row r="63" spans="8:26" x14ac:dyDescent="0.25">
@@ -11740,27 +10866,27 @@
       </c>
       <c r="L64" s="3">
         <f>AVERAGE(K$1:K$3)</f>
-        <v>0.99323518767684849</v>
+        <v>0.9932352089703107</v>
       </c>
       <c r="M64" s="3">
         <f>AVERAGE(K$4:K$6)</f>
-        <v>0.99460152470338004</v>
+        <v>0.99460154687993896</v>
       </c>
       <c r="N64" s="3">
         <f>AVERAGE(K$7:K$12,K$17:K$19)</f>
-        <v>0.9898081646470942</v>
+        <v>0.98980700276706002</v>
       </c>
       <c r="O64" s="3">
         <f>AVERAGE(K$13:K$16)</f>
-        <v>0.99704846735571739</v>
+        <v>0.99704870081823149</v>
       </c>
       <c r="P64" s="3">
         <f>K$20</f>
-        <v>0.99429033921516119</v>
+        <v>0.99428979846547727</v>
       </c>
       <c r="Q64" s="3">
         <f>AVERAGE(K$21:K$22)</f>
-        <v>0.99053306978619449</v>
+        <v>0.99053303382368307</v>
       </c>
       <c r="U64" t="str">
         <f>_xlfn.CONCAT(ROUND(L64,2), " ± ", L65)</f>
@@ -11831,27 +10957,27 @@
       </c>
       <c r="M68" s="3">
         <f>AVERAGE(L$1:L$3)</f>
-        <v>0.98263029317179151</v>
+        <v>0.98300514614760737</v>
       </c>
       <c r="N68">
         <f>AVERAGE(L$4:L$6)</f>
-        <v>0.96424374674301827</v>
+        <v>0.96470484724003958</v>
       </c>
       <c r="O68">
         <f>AVERAGE(L$7:L$12,L$17:L$19)</f>
-        <v>0.96715093632453075</v>
+        <v>0.96747248940537267</v>
       </c>
       <c r="P68">
         <f>AVERAGE(L$13:L$16)</f>
-        <v>0.98477732736147738</v>
+        <v>0.98513044742139777</v>
       </c>
       <c r="Q68">
         <f>L$20</f>
-        <v>0.99110919057621594</v>
+        <v>0.99141974525984633</v>
       </c>
       <c r="R68">
         <f>AVERAGE(L$21:L$22)</f>
-        <v>0.9593689558297307</v>
+        <v>0.95949525542250658</v>
       </c>
       <c r="V68" t="str">
         <f>_xlfn.CONCAT(ROUND(M68,2), " ± ", M69)</f>
@@ -11867,7 +10993,7 @@
       </c>
       <c r="Y68" t="str">
         <f t="shared" ref="Y68" si="15">_xlfn.CONCAT(ROUND(P68,2), " ± ", P69)</f>
-        <v>0.98 ± 6.99E-03</v>
+        <v>0.99 ± 6.99E-03</v>
       </c>
       <c r="Z68" t="str">
         <f t="shared" ref="Z68" si="16">_xlfn.CONCAT(ROUND(Q68,2), " ± ", Q69)</f>
@@ -11922,27 +11048,27 @@
       </c>
       <c r="N72">
         <f>AVERAGE(M$1:M$3)</f>
-        <v>0.98530636450758013</v>
+        <v>0.98559997593529081</v>
       </c>
       <c r="O72">
         <f>AVERAGE(M$4:M$6)</f>
-        <v>0.96919058691022419</v>
+        <v>0.9693800503323432</v>
       </c>
       <c r="P72">
         <f>AVERAGE(M$7:M$12,M$17:M$19)</f>
-        <v>0.98255846735418551</v>
+        <v>0.98251601658270615</v>
       </c>
       <c r="Q72">
         <f>AVERAGE(M$13:M$16)</f>
-        <v>0.97161338595597191</v>
+        <v>0.97197594133035303</v>
       </c>
       <c r="R72">
         <f>M$20</f>
-        <v>0.98947858595712912</v>
+        <v>0.99018690753118732</v>
       </c>
       <c r="S72">
         <f>AVERAGE(M$21:M$22)</f>
-        <v>0.98682147295959011</v>
+        <v>0.98683977489400232</v>
       </c>
       <c r="W72" t="str">
         <f>_xlfn.CONCAT(ROUND(N72,2), " ± ", N73)</f>
@@ -12013,27 +11139,27 @@
       </c>
       <c r="O76">
         <f>AVERAGE(N$1:N$3)</f>
-        <v>8.0362220674373541E-2</v>
+        <v>8.0362041918497926E-2</v>
       </c>
       <c r="P76">
         <f>AVERAGE(N$4:N$6)</f>
-        <v>7.2878491447742999E-2</v>
+        <v>7.2878411067648224E-2</v>
       </c>
       <c r="Q76">
         <f>AVERAGE(N$7:N$12,N$17:N$19)</f>
-        <v>9.0546510734779762E-2</v>
+        <v>9.0554912863946804E-2</v>
       </c>
       <c r="R76">
         <f>AVERAGE(N$13:N$16)</f>
-        <v>5.1210346785538013E-2</v>
+        <v>5.1207290162989402E-2</v>
       </c>
       <c r="S76">
         <f>N$20</f>
-        <v>7.5183536608691551E-2</v>
+        <v>7.5187096759866429E-2</v>
       </c>
       <c r="T76">
         <f>AVERAGE(N$21:N$22)</f>
-        <v>9.6647862860316569E-2</v>
+        <v>9.6648036792624958E-2</v>
       </c>
       <c r="X76" t="str">
         <f>_xlfn.CONCAT(ROUND(O76,2), " ± ", O77)</f>
@@ -12104,27 +11230,27 @@
       </c>
       <c r="P80">
         <f>AVERAGE(O$1:O$3)</f>
-        <v>0.13101615036119504</v>
+        <v>0.12957358367758393</v>
       </c>
       <c r="Q80">
         <f>AVERAGE(O$4:O$6)</f>
-        <v>0.17944891413819461</v>
+        <v>0.17825620245069648</v>
       </c>
       <c r="R80">
         <f>AVERAGE(O$7:O$12,O$17:O$19)</f>
-        <v>0.16477034356947898</v>
+        <v>0.16358160762849916</v>
       </c>
       <c r="S80">
         <f>AVERAGE(O$13:O$16)</f>
-        <v>0.11456741663886996</v>
+        <v>0.11256860779181954</v>
       </c>
       <c r="T80">
         <f>O$20</f>
-        <v>9.3818448769665122E-2</v>
+        <v>9.2165352452817859E-2</v>
       </c>
       <c r="U80">
         <f>AVERAGE(O$21:O$22)</f>
-        <v>0.1932442823935604</v>
+        <v>0.19280785775103676</v>
       </c>
       <c r="Y80" t="str">
         <f>_xlfn.CONCAT(ROUND(P80,2), " ± ", P81)</f>
@@ -12195,27 +11321,27 @@
       </c>
       <c r="Q84">
         <f>AVERAGE(P$1:P$3)</f>
-        <v>0.11142200419504411</v>
+        <v>0.11022569489394717</v>
       </c>
       <c r="R84">
         <f>AVERAGE(P$4:P$6)</f>
-        <v>0.16245718660048794</v>
+        <v>0.16197315664774298</v>
       </c>
       <c r="S84">
         <f>AVERAGE(P$7:P$12,P$17:P$19)</f>
-        <v>0.11893605064820632</v>
+        <v>0.11909202014710722</v>
       </c>
       <c r="T84">
         <f>AVERAGE(P$13:P$16)</f>
-        <v>0.14289996483129169</v>
+        <v>0.14164597265955758</v>
       </c>
       <c r="U84">
         <f>P$20</f>
-        <v>0.10205978592198878</v>
+        <v>9.8564504483736548E-2</v>
       </c>
       <c r="V84">
         <f>AVERAGE(P$21:P$22)</f>
-        <v>0.11176121421762646</v>
+        <v>0.11172157128821517</v>
       </c>
       <c r="Z84" t="str">
         <f>_xlfn.CONCAT(ROUND(Q84,2), " ± ", Q85)</f>
@@ -12286,50 +11412,50 @@
       </c>
       <c r="R88" s="2">
         <f>AVERAGE(Q$1:Q$3)</f>
-        <v>2.037862058825092E-2</v>
+        <v>2.0365681512952261E-2</v>
       </c>
       <c r="S88" s="2">
         <f>AVERAGE(Q$4:Q$6)</f>
-        <v>1.9912909647962457E-2</v>
+        <v>1.9902792231451975E-2</v>
       </c>
       <c r="T88" s="2">
         <f>AVERAGE(Q$7:Q$12,Q$17:Q$19)</f>
-        <v>2.0515103427541762E-2</v>
+        <v>2.0561912508965351E-2</v>
       </c>
       <c r="U88" s="2">
         <f>AVERAGE(Q$13:Q$16)</f>
-        <v>2.0409427432635803E-2</v>
+        <v>2.0431830067845134E-2</v>
       </c>
       <c r="V88" s="2">
         <f>Q$20</f>
-        <v>2.0902529677286813E-2</v>
+        <v>2.0784713283118691E-2</v>
       </c>
       <c r="W88" s="2">
         <f>AVERAGE(Q$21:Q$22)</f>
-        <v>2.068643633958234E-2</v>
+        <v>2.0754795921728013E-2</v>
       </c>
     </row>
     <row r="89" spans="16:31" x14ac:dyDescent="0.25">
       <c r="R89" s="2">
         <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
-        <v>3.8905919800278743E-4</v>
+        <v>3.8194997275177109E-4</v>
       </c>
       <c r="S89" s="2">
         <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
-        <v>3.0506651067963139E-4</v>
+        <v>2.9494907968756836E-4</v>
       </c>
       <c r="T89" s="2">
         <f>STDEV(Q$7:Q$12,Q$17:Q$19)/SQRT(COUNT(Q$7:Q$12,Q$17:Q$19))</f>
-        <v>2.1590559082891949E-4</v>
+        <v>2.310682053692697E-4</v>
       </c>
       <c r="U89" s="2">
         <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
-        <v>4.6278990617203001E-4</v>
+        <v>4.7544596282562859E-4</v>
       </c>
       <c r="V89" s="2"/>
       <c r="W89" s="2">
         <f>STDEV(Q$21:Q$22)/SQRT(COUNT(Q$21:Q$22))</f>
-        <v>9.8987882803977523E-5</v>
+        <v>1.7933404971992757E-4</v>
       </c>
     </row>
     <row r="91" spans="16:31" x14ac:dyDescent="0.25">
@@ -12358,76 +11484,76 @@
       </c>
       <c r="S92" s="2">
         <f>AVERAGE(R$1:R$3)</f>
-        <v>2.6626665084659509E-2</v>
+        <v>2.6578997644427605E-2</v>
       </c>
       <c r="T92" s="2">
         <f>AVERAGE(R$4:R$6)</f>
-        <v>2.678220265577928E-2</v>
+        <v>2.6835872828472173E-2</v>
       </c>
       <c r="U92" s="2">
         <f>AVERAGE(R$7:R$12,R$17:R$19)</f>
-        <v>2.6913361518582011E-2</v>
+        <v>2.6886662268571313E-2</v>
       </c>
       <c r="V92" s="2">
         <f>AVERAGE(R$13:R$16)</f>
-        <v>2.6763462286901768E-2</v>
+        <v>2.6657237171290454E-2</v>
       </c>
       <c r="W92" s="2">
         <f>R$20</f>
-        <v>2.6623766806585347E-2</v>
+        <v>2.6593421852223683E-2</v>
       </c>
       <c r="X92" s="2">
         <f>AVERAGE(R$21:R$22)</f>
-        <v>2.6746041579962625E-2</v>
+        <v>2.6777762541119757E-2</v>
       </c>
     </row>
     <row r="93" spans="16:31" x14ac:dyDescent="0.25">
       <c r="S93" s="2">
         <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
-        <v>6.790444705159948E-5</v>
+        <v>2.1625069528551808E-5</v>
       </c>
       <c r="T93" s="2">
         <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
-        <v>7.4724977136014664E-5</v>
+        <v>4.8710360305349656E-5</v>
       </c>
       <c r="U93" s="2">
         <f>STDEV(R$7:R$12,R$17:R$19)/SQRT(COUNT(R$7:R$12,R$17:R$19))</f>
-        <v>1.6268316449898223E-4</v>
+        <v>1.614486351023254E-4</v>
       </c>
       <c r="V93" s="2">
         <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
-        <v>1.9335632166111503E-4</v>
+        <v>1.279616788292203E-4</v>
       </c>
       <c r="W93" s="2"/>
       <c r="X93" s="2">
         <f>STDEV(R$21:R$22)/SQRT(COUNT(R$21:R$22))</f>
-        <v>2.7860731561090558E-6</v>
+        <v>2.9679016567189798E-5</v>
       </c>
     </row>
     <row r="99" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S99" s="3">
         <f>1/S92</f>
-        <v>37.556336733139467</v>
+        <v>37.623691208297089</v>
       </c>
       <c r="T99" s="3">
         <f t="shared" ref="T99:X99" si="38">1/T92</f>
-        <v>37.338228406848827</v>
+        <v>37.263554138586677</v>
       </c>
       <c r="U99" s="3">
         <f t="shared" si="38"/>
-        <v>37.1562652740187</v>
+        <v>37.193162543233647</v>
       </c>
       <c r="V99" s="3">
         <f t="shared" si="38"/>
-        <v>37.364373461105117</v>
+        <v>37.513264918428561</v>
       </c>
       <c r="W99" s="3">
         <f t="shared" si="38"/>
-        <v>37.560425136861234</v>
+        <v>37.603284209037668</v>
       </c>
       <c r="X99" s="3">
         <f t="shared" si="38"/>
-        <v>37.388710288597309</v>
+        <v>37.344419589366609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actually, the kMCT4 trend is gone after having changed both of them
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox_moredata.xlsx
+++ b/Lacex_summary_hptoolbox_moredata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFB8210-0E6A-4AAD-B239-3F2ECBD7AC90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26611F46-756B-4F7A-B2A5-D1E5AC582B35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A183822-7954-4BE4-BDAB-B5FAE4C8B5A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Old Tableized Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="178">
   <si>
     <t>HK-2</t>
   </si>
@@ -567,96 +568,6 @@
   </si>
   <si>
     <t>1.64E-01 ± 1.89E-02</t>
-  </si>
-  <si>
-    <t>3.94E-07 ± 3.94E-07</t>
-  </si>
-  <si>
-    <t>1.65E-03</t>
-  </si>
-  <si>
-    <t>5.99E-04</t>
-  </si>
-  <si>
-    <t>3.55E-03</t>
-  </si>
-  <si>
-    <t>1.16E-03</t>
-  </si>
-  <si>
-    <t>1.10E-03</t>
-  </si>
-  <si>
-    <t>1.11E-03</t>
-  </si>
-  <si>
-    <t>1.49E-02</t>
-  </si>
-  <si>
-    <t>9.00E-03</t>
-  </si>
-  <si>
-    <t>6.99E-03</t>
-  </si>
-  <si>
-    <t>2.11E-02</t>
-  </si>
-  <si>
-    <t>8.28E-03</t>
-  </si>
-  <si>
-    <t>1.64E-02</t>
-  </si>
-  <si>
-    <t>6.39E-03</t>
-  </si>
-  <si>
-    <t>1.96E-02</t>
-  </si>
-  <si>
-    <t>5.28E-03</t>
-  </si>
-  <si>
-    <t>1.09E-02</t>
-  </si>
-  <si>
-    <t>4.07E-03</t>
-  </si>
-  <si>
-    <t>1.54E-02</t>
-  </si>
-  <si>
-    <t>9.99E-03</t>
-  </si>
-  <si>
-    <t>5.61E-03</t>
-  </si>
-  <si>
-    <t>4.22E-03</t>
-  </si>
-  <si>
-    <t>3.98E-02</t>
-  </si>
-  <si>
-    <t>2.61E-02</t>
-  </si>
-  <si>
-    <t>5.41E-02</t>
-  </si>
-  <si>
-    <t>3.25E-02</t>
-  </si>
-  <si>
-    <t>4.52E-02</t>
-  </si>
-  <si>
-    <t>1.98E-02</t>
-  </si>
-  <si>
-    <t>5.06E-02</t>
-  </si>
-  <si>
-    <t>2.34E-02</t>
   </si>
 </sst>
 </file>
@@ -7334,16 +7245,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>676548</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>90896</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>482510</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>415290</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>502376</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>167096</xdr:rowOff>
+      <xdr:rowOff>40277</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7672,7 +7583,7 @@
   <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="S93" sqref="S93:X93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10888,19 +10799,19 @@
       </c>
       <c r="U64" t="str">
         <f>_xlfn.CONCAT(ROUND(L64,2), " ± ", L65)</f>
-        <v>0.99 ± 1.65E-03</v>
+        <v>0.99 ± 0.00164637145107342</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" ref="V64:Z64" si="12">_xlfn.CONCAT(ROUND(M64,2), " ± ", M65)</f>
-        <v>0.99 ± 5.99E-04</v>
+        <v>0.99 ± 0.000615872929178806</v>
       </c>
       <c r="W64" t="str">
         <f t="shared" si="12"/>
-        <v>0.99 ± 3.55E-03</v>
+        <v>0.99 ± 0.00354879781997329</v>
       </c>
       <c r="X64" t="str">
         <f t="shared" si="12"/>
-        <v>1 ± 1.16E-03</v>
+        <v>1 ± 0.00115539480497226</v>
       </c>
       <c r="Y64" t="str">
         <f t="shared" si="12"/>
@@ -10908,25 +10819,30 @@
       </c>
       <c r="Z64" t="str">
         <f t="shared" si="12"/>
-        <v>0.99 ± 1.10E-03</v>
+        <v>0.99 ± 0.00109502059391814</v>
       </c>
     </row>
     <row r="65" spans="12:30" x14ac:dyDescent="0.25">
-      <c r="L65" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M65" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="N65" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="4" t="s">
-        <v>183</v>
+      <c r="L65" s="2">
+        <f>STDEV(K$1:K$3)/SQRT(COUNT(K$1:K$3))</f>
+        <v>1.6463714510734249E-3</v>
+      </c>
+      <c r="M65" s="2">
+        <f>STDEV(K$4:K$6)/SQRT(COUNT(K$4:K$6))</f>
+        <v>6.1587292917880557E-4</v>
+      </c>
+      <c r="N65" s="2">
+        <f>STDEV(K$7:K$12,K$17:K$19)/SQRT(COUNT(K$7:K$12,K$17:K$19))</f>
+        <v>3.5487978199732939E-3</v>
+      </c>
+      <c r="O65" s="2">
+        <f>STDEV(K$13:K$16)/SQRT(COUNT(K$13:K$16))</f>
+        <v>1.1553948049722602E-3</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2">
+        <f>STDEV(K$21:K$22)/SQRT(COUNT(K$21:K$22))</f>
+        <v>1.095020593918139E-3</v>
       </c>
     </row>
     <row r="67" spans="12:30" x14ac:dyDescent="0.25">
@@ -10979,19 +10895,19 @@
       </c>
       <c r="V68" t="str">
         <f>_xlfn.CONCAT(ROUND(M68,2), " ± ", M69)</f>
-        <v>0.98 ± 1.11E-03</v>
+        <v>0.98 ± 0.00371948411285703</v>
       </c>
       <c r="W68" t="str">
         <f t="shared" ref="W68" si="13">_xlfn.CONCAT(ROUND(N68,2), " ± ", N69)</f>
-        <v>0.96 ± 1.49E-02</v>
+        <v>0.96 ± 0.0208296495059325</v>
       </c>
       <c r="X68" t="str">
         <f t="shared" ref="X68" si="14">_xlfn.CONCAT(ROUND(O68,2), " ± ", O69)</f>
-        <v>0.96 ± 9.00E-03</v>
+        <v>0.96 ± 0.010159758260436</v>
       </c>
       <c r="Y68" t="str">
         <f t="shared" ref="Y68" si="15">_xlfn.CONCAT(ROUND(P68,2), " ± ", P69)</f>
-        <v>0.98 ± 6.99E-03</v>
+        <v>0.98 ± 0.00766709511288894</v>
       </c>
       <c r="Z68" t="str">
         <f t="shared" ref="Z68" si="16">_xlfn.CONCAT(ROUND(Q68,2), " ± ", Q69)</f>
@@ -10999,25 +10915,30 @@
       </c>
       <c r="AA68" t="str">
         <f t="shared" ref="AA68" si="17">_xlfn.CONCAT(ROUND(R68,2), " ± ", R69)</f>
-        <v>0.96 ± 2.11E-02</v>
+        <v>0.96 ± 0.0210693425232379</v>
       </c>
     </row>
     <row r="69" spans="12:30" x14ac:dyDescent="0.25">
-      <c r="M69" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="N69" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="O69" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="P69" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q69" s="3"/>
-      <c r="R69" s="4" t="s">
-        <v>188</v>
+      <c r="M69" s="2">
+        <f>STDEV(L$1:L$3)/SQRT(COUNT(L$1:L$3))</f>
+        <v>3.7194841128570279E-3</v>
+      </c>
+      <c r="N69" s="2">
+        <f>STDEV(L$4:L$6)/SQRT(COUNT(L$4:L$6))</f>
+        <v>2.0829649505932534E-2</v>
+      </c>
+      <c r="O69" s="2">
+        <f>STDEV(L$7:L$12,L$17:L$19)/SQRT(COUNT(L$7:L$12,L$17:L$19))</f>
+        <v>1.0159758260436006E-2</v>
+      </c>
+      <c r="P69" s="2">
+        <f>STDEV(L$13:L$16)/SQRT(COUNT(L$13:L$16))</f>
+        <v>7.6670951128889392E-3</v>
+      </c>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2">
+        <f>STDEV(L$21:L$22)/SQRT(COUNT(L$21:L$22))</f>
+        <v>2.106934252323794E-2</v>
       </c>
     </row>
     <row r="71" spans="12:30" x14ac:dyDescent="0.25">
@@ -11070,19 +10991,19 @@
       </c>
       <c r="W72" t="str">
         <f>_xlfn.CONCAT(ROUND(N72,2), " ± ", N73)</f>
-        <v>0.99 ± 8.28E-03</v>
+        <v>0.99 ± 0.0081010346831268</v>
       </c>
       <c r="X72" t="str">
         <f t="shared" ref="X72" si="18">_xlfn.CONCAT(ROUND(O72,2), " ± ", O73)</f>
-        <v>0.95 ± 1.64E-02</v>
+        <v>0.95 ± 0.031689735417869</v>
       </c>
       <c r="Y72" t="str">
         <f t="shared" ref="Y72" si="19">_xlfn.CONCAT(ROUND(P72,2), " ± ", P73)</f>
-        <v>0.98 ± 6.39E-03</v>
+        <v>0.98 ± 0.0068300721229364</v>
       </c>
       <c r="Z72" t="str">
         <f t="shared" ref="Z72" si="20">_xlfn.CONCAT(ROUND(Q72,2), " ± ", Q73)</f>
-        <v>0.98 ± 1.96E-02</v>
+        <v>0.98 ± 0.0149382572576369</v>
       </c>
       <c r="AA72" t="str">
         <f t="shared" ref="AA72" si="21">_xlfn.CONCAT(ROUND(R72,2), " ± ", R73)</f>
@@ -11090,25 +11011,30 @@
       </c>
       <c r="AB72" t="str">
         <f t="shared" ref="AB72" si="22">_xlfn.CONCAT(ROUND(S72,2), " ± ", S73)</f>
-        <v>0.99 ± 5.28E-03</v>
+        <v>0.99 ± 0.00528473818054187</v>
       </c>
     </row>
     <row r="73" spans="12:30" x14ac:dyDescent="0.25">
-      <c r="N73" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="O73" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="P73" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q73" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="R73" s="3"/>
-      <c r="S73" s="4" t="s">
-        <v>193</v>
+      <c r="N73" s="2">
+        <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
+        <v>8.1010346831268017E-3</v>
+      </c>
+      <c r="O73" s="2">
+        <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
+        <v>3.1689735417869021E-2</v>
+      </c>
+      <c r="P73" s="2">
+        <f>STDEV(M$7:M$12,M$17:M$19)/SQRT(COUNT(M$7:M$12,M$17:M$19))</f>
+        <v>6.8300721229363993E-3</v>
+      </c>
+      <c r="Q73" s="2">
+        <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
+        <v>1.4938257257636881E-2</v>
+      </c>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2">
+        <f>STDEV(M$21:M$22)/SQRT(COUNT(M$21:M$22))</f>
+        <v>5.2847381805418703E-3</v>
       </c>
     </row>
     <row r="75" spans="12:30" x14ac:dyDescent="0.25">
@@ -11161,19 +11087,19 @@
       </c>
       <c r="X76" t="str">
         <f>_xlfn.CONCAT(ROUND(O76,2), " ± ", O77)</f>
-        <v>0.08 ± 1.09E-02</v>
+        <v>0.08 ± 0.0108642478170271</v>
       </c>
       <c r="Y76" t="str">
         <f t="shared" ref="Y76" si="23">_xlfn.CONCAT(ROUND(P76,2), " ± ", P77)</f>
-        <v>0.07 ± 4.07E-03</v>
+        <v>0.07 ± 0.00415022803225121</v>
       </c>
       <c r="Z76" t="str">
         <f t="shared" ref="Z76" si="24">_xlfn.CONCAT(ROUND(Q76,2), " ± ", Q77)</f>
-        <v>0.09 ± 1.54E-02</v>
+        <v>0.09 ± 0.0153681447026587</v>
       </c>
       <c r="AA76" t="str">
         <f t="shared" ref="AA76" si="25">_xlfn.CONCAT(ROUND(R76,2), " ± ", R77)</f>
-        <v>0.05 ± 9.99E-03</v>
+        <v>0.05 ± 0.00989083967946045</v>
       </c>
       <c r="AB76" t="str">
         <f t="shared" ref="AB76" si="26">_xlfn.CONCAT(ROUND(S76,2), " ± ", S77)</f>
@@ -11181,25 +11107,30 @@
       </c>
       <c r="AC76" t="str">
         <f t="shared" ref="AC76" si="27">_xlfn.CONCAT(ROUND(T76,2), " ± ", T77)</f>
-        <v>0.1 ± 5.61E-03</v>
+        <v>0.1 ± 0.00560834147911541</v>
       </c>
     </row>
     <row r="77" spans="12:30" x14ac:dyDescent="0.25">
-      <c r="O77" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="P77" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q77" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="R77" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="S77" s="3"/>
-      <c r="T77" s="4" t="s">
-        <v>198</v>
+      <c r="O77" s="2">
+        <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
+        <v>1.0864247817027092E-2</v>
+      </c>
+      <c r="P77" s="2">
+        <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
+        <v>4.1502280322512136E-3</v>
+      </c>
+      <c r="Q77" s="2">
+        <f>STDEV(N$7:N$12,N$17:N$19)/SQRT(COUNT(N$7:N$12,N$17:N$19))</f>
+        <v>1.536814470265868E-2</v>
+      </c>
+      <c r="R77" s="2">
+        <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
+        <v>9.8908396794604517E-3</v>
+      </c>
+      <c r="S77" s="2"/>
+      <c r="T77" s="2">
+        <f>STDEV(N$21:N$22)/SQRT(COUNT(N$21:N$22))</f>
+        <v>5.6083414791154107E-3</v>
       </c>
     </row>
     <row r="79" spans="12:30" x14ac:dyDescent="0.25">
@@ -11252,19 +11183,19 @@
       </c>
       <c r="Y80" t="str">
         <f>_xlfn.CONCAT(ROUND(P80,2), " ± ", P81)</f>
-        <v>0.14 ± 4.22E-03</v>
+        <v>0.14 ± 0.0127564831231008</v>
       </c>
       <c r="Z80" t="str">
         <f t="shared" ref="Z80" si="28">_xlfn.CONCAT(ROUND(Q80,2), " ± ", Q81)</f>
-        <v>0.19 ± 3.98E-02</v>
+        <v>0.19 ± 0.0484165940329263</v>
       </c>
       <c r="AA80" t="str">
         <f t="shared" ref="AA80" si="29">_xlfn.CONCAT(ROUND(R80,2), " ± ", R81)</f>
-        <v>0.17 ± 2.61E-02</v>
+        <v>0.17 ± 0.0280719074671355</v>
       </c>
       <c r="AB80" t="str">
         <f t="shared" ref="AB80" si="30">_xlfn.CONCAT(ROUND(S80,2), " ± ", S81)</f>
-        <v>0.12 ± 2.61E-02</v>
+        <v>0.12 ± 0.0281202696662261</v>
       </c>
       <c r="AC80" t="str">
         <f t="shared" ref="AC80" si="31">_xlfn.CONCAT(ROUND(T80,2), " ± ", T81)</f>
@@ -11272,25 +11203,30 @@
       </c>
       <c r="AD80" t="str">
         <f t="shared" ref="AD80" si="32">_xlfn.CONCAT(ROUND(U80,2), " ± ", U81)</f>
-        <v>0.19 ± 5.41E-02</v>
+        <v>0.19 ± 0.0540895871224242</v>
       </c>
     </row>
     <row r="81" spans="16:31" x14ac:dyDescent="0.25">
-      <c r="P81" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q81" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="R81" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="S81" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="T81" s="3"/>
-      <c r="U81" s="4" t="s">
-        <v>202</v>
+      <c r="P81" s="2">
+        <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
+        <v>1.2756483123100756E-2</v>
+      </c>
+      <c r="Q81" s="2">
+        <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
+        <v>4.8416594032926287E-2</v>
+      </c>
+      <c r="R81" s="2">
+        <f>STDEV(O$7:O$12,O$17:O$19)/SQRT(COUNT(O$7:O$12,O$17:O$19))</f>
+        <v>2.8071907467135549E-2</v>
+      </c>
+      <c r="S81" s="2">
+        <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
+        <v>2.8120269666226067E-2</v>
+      </c>
+      <c r="T81" s="2"/>
+      <c r="U81" s="2">
+        <f>STDEV(O$21:O$22)/SQRT(COUNT(O$21:O$22))</f>
+        <v>5.4089587122424169E-2</v>
       </c>
     </row>
     <row r="83" spans="16:31" x14ac:dyDescent="0.25">
@@ -11343,19 +11279,19 @@
       </c>
       <c r="Z84" t="str">
         <f>_xlfn.CONCAT(ROUND(Q84,2), " ± ", Q85)</f>
-        <v>0.11 ± 3.25E-02</v>
+        <v>0.11 ± 0.031298052001519</v>
       </c>
       <c r="AA84" t="str">
         <f t="shared" ref="AA84" si="33">_xlfn.CONCAT(ROUND(R84,2), " ± ", R85)</f>
-        <v>0.21 ± 4.52E-02</v>
+        <v>0.21 ± 0.0656382800118405</v>
       </c>
       <c r="AB84" t="str">
         <f t="shared" ref="AB84" si="34">_xlfn.CONCAT(ROUND(S84,2), " ± ", S85)</f>
-        <v>0.13 ± 1.98E-02</v>
+        <v>0.13 ± 0.0213828634553278</v>
       </c>
       <c r="AC84" t="str">
         <f t="shared" ref="AC84" si="35">_xlfn.CONCAT(ROUND(T84,2), " ± ", T85)</f>
-        <v>0.13 ± 5.06E-02</v>
+        <v>0.13 ± 0.0426346878237909</v>
       </c>
       <c r="AD84" t="str">
         <f t="shared" ref="AD84" si="36">_xlfn.CONCAT(ROUND(U84,2), " ± ", U85)</f>
@@ -11363,25 +11299,30 @@
       </c>
       <c r="AE84" t="str">
         <f t="shared" ref="AE84" si="37">_xlfn.CONCAT(ROUND(V84,2), " ± ", V85)</f>
-        <v>0.11 ± 2.34E-02</v>
+        <v>0.11 ± 0.023422468099409</v>
       </c>
     </row>
     <row r="85" spans="16:31" x14ac:dyDescent="0.25">
-      <c r="Q85" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="R85" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="S85" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="T85" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="U85" s="3"/>
-      <c r="V85" s="4" t="s">
-        <v>207</v>
+      <c r="Q85" s="2">
+        <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
+        <v>3.1298052001519007E-2</v>
+      </c>
+      <c r="R85" s="2">
+        <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
+        <v>6.563828001184048E-2</v>
+      </c>
+      <c r="S85" s="2">
+        <f>STDEV(P$7:P$12,P$17:P$19)/SQRT(COUNT(P$7:P$12,P$17:P$19))</f>
+        <v>2.1382863455327823E-2</v>
+      </c>
+      <c r="T85" s="2">
+        <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
+        <v>4.263468782379095E-2</v>
+      </c>
+      <c r="U85" s="2"/>
+      <c r="V85" s="2">
+        <f>STDEV(P$21:P$22)/SQRT(COUNT(P$21:P$22))</f>
+        <v>2.3422468099408952E-2</v>
       </c>
     </row>
     <row r="87" spans="16:31" x14ac:dyDescent="0.25">
@@ -11608,12 +11549,756 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B6BAAC-6A3E-4E58-9981-CF1298A0FB5A}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.1001291329547363E-3</v>
+      </c>
+      <c r="B2">
+        <v>9.2818145298093388E-2</v>
+      </c>
+      <c r="C2">
+        <v>5.0868748663837837E-2</v>
+      </c>
+      <c r="D2">
+        <v>633622671.09765995</v>
+      </c>
+      <c r="E2">
+        <v>20.597155249553094</v>
+      </c>
+      <c r="F2">
+        <v>63.472995846278707</v>
+      </c>
+      <c r="G2">
+        <v>0.43346035797148019</v>
+      </c>
+      <c r="H2">
+        <v>3.6286411899082473E-2</v>
+      </c>
+      <c r="I2">
+        <v>3.3953097177711229E-3</v>
+      </c>
+      <c r="J2">
+        <v>3.3333430095271155E-3</v>
+      </c>
+      <c r="K2">
+        <v>0.99322700086671922</v>
+      </c>
+      <c r="L2">
+        <v>0.98035097498913748</v>
+      </c>
+      <c r="M2">
+        <v>0.98523464208513778</v>
+      </c>
+      <c r="N2">
+        <v>8.043137062544925E-2</v>
+      </c>
+      <c r="O2">
+        <v>0.13830068343075549</v>
+      </c>
+      <c r="P2">
+        <v>0.1125103027172797</v>
+      </c>
+      <c r="Q2">
+        <v>2.0542256242548931E-2</v>
+      </c>
+      <c r="R2">
+        <v>2.6564180849319923E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6.6344325228484607E-3</v>
+      </c>
+      <c r="B3">
+        <v>0.43188845352491184</v>
+      </c>
+      <c r="C3">
+        <v>5.0864252470759146E-2</v>
+      </c>
+      <c r="D3">
+        <v>429431962.72254306</v>
+      </c>
+      <c r="E3">
+        <v>22.151515922238428</v>
+      </c>
+      <c r="F3">
+        <v>61.889515079945674</v>
+      </c>
+      <c r="G3">
+        <v>0.196532097703467</v>
+      </c>
+      <c r="H3">
+        <v>0.26385942952199509</v>
+      </c>
+      <c r="I3">
+        <v>8.8282120593786674E-7</v>
+      </c>
+      <c r="J3">
+        <v>8.929136820414128E-3</v>
+      </c>
+      <c r="K3">
+        <v>0.9945440842781158</v>
+      </c>
+      <c r="L3">
+        <v>0.9579250882516176</v>
+      </c>
+      <c r="M3">
+        <v>0.94752711607979234</v>
+      </c>
+      <c r="N3">
+        <v>7.3259182217835686E-2</v>
+      </c>
+      <c r="O3">
+        <v>0.1922649980506077</v>
+      </c>
+      <c r="P3">
+        <v>0.20816192609403875</v>
+      </c>
+      <c r="Q3">
+        <v>1.9975193205712585E-2</v>
+      </c>
+      <c r="R3">
+        <v>2.6892349117898989E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.8632184488774763E-2</v>
+      </c>
+      <c r="B4">
+        <v>0.2344887167481633</v>
+      </c>
+      <c r="C4">
+        <v>6.9876411281357811E-2</v>
+      </c>
+      <c r="D4">
+        <v>670372763.92028725</v>
+      </c>
+      <c r="E4">
+        <v>27.065332195618783</v>
+      </c>
+      <c r="F4">
+        <v>62.701474248091728</v>
+      </c>
+      <c r="G4">
+        <v>0.43023011394463978</v>
+      </c>
+      <c r="H4">
+        <v>0.31383707412990214</v>
+      </c>
+      <c r="I4">
+        <v>1.1209793148765927E-3</v>
+      </c>
+      <c r="J4">
+        <v>2.8879858594523015E-3</v>
+      </c>
+      <c r="K4">
+        <v>0.98980424274963696</v>
+      </c>
+      <c r="L4">
+        <v>0.96410488144668505</v>
+      </c>
+      <c r="M4">
+        <v>0.98013828000277081</v>
+      </c>
+      <c r="N4">
+        <v>9.057807874384223E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.17097358363780107</v>
+      </c>
+      <c r="P4">
+        <v>0.12651233838552542</v>
+      </c>
+      <c r="Q4">
+        <v>2.0633748084395762E-2</v>
+      </c>
+      <c r="R4">
+        <v>2.6960438882680453E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.217832001894262E-3</v>
+      </c>
+      <c r="B5">
+        <v>7.9975010194079946E-2</v>
+      </c>
+      <c r="C5">
+        <v>7.455669266619476E-2</v>
+      </c>
+      <c r="D5">
+        <v>1129232402.7311361</v>
+      </c>
+      <c r="E5">
+        <v>30.483055442493249</v>
+      </c>
+      <c r="F5">
+        <v>62.632868531488306</v>
+      </c>
+      <c r="G5">
+        <v>0.35208886709488357</v>
+      </c>
+      <c r="H5">
+        <v>0.26062308636909265</v>
+      </c>
+      <c r="I5">
+        <v>2.4831981979508257E-3</v>
+      </c>
+      <c r="J5">
+        <v>5.0330206765200215E-3</v>
+      </c>
+      <c r="K5">
+        <v>0.99703384835239794</v>
+      </c>
+      <c r="L5">
+        <v>0.9834694816438827</v>
+      </c>
+      <c r="M5">
+        <v>0.97698140406207412</v>
+      </c>
+      <c r="N5">
+        <v>5.1410154662592682E-2</v>
+      </c>
+      <c r="O5">
+        <v>0.11829186140327759</v>
+      </c>
+      <c r="P5">
+        <v>0.1316634351710842</v>
+      </c>
+      <c r="Q5">
+        <v>2.0435630269480996E-2</v>
+      </c>
+      <c r="R5">
+        <v>2.690102607904258E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.0759029324079272E-2</v>
+      </c>
+      <c r="B6">
+        <v>0.10806440153231296</v>
+      </c>
+      <c r="C6">
+        <v>9.9999999999865849E-2</v>
+      </c>
+      <c r="D6">
+        <v>1442195507.9818859</v>
+      </c>
+      <c r="E6">
+        <v>21.071899069677666</v>
+      </c>
+      <c r="F6">
+        <v>66.224948294347939</v>
+      </c>
+      <c r="G6">
+        <v>0.64161205898035911</v>
+      </c>
+      <c r="H6">
+        <v>0.11940514825193088</v>
+      </c>
+      <c r="I6">
+        <v>2.843330400548159E-12</v>
+      </c>
+      <c r="J6">
+        <v>9.9999988405638767E-3</v>
+      </c>
+      <c r="K6">
+        <v>0.99428979830560293</v>
+      </c>
+      <c r="L6">
+        <v>0.99141732978265473</v>
+      </c>
+      <c r="M6">
+        <v>0.99019570580954175</v>
+      </c>
+      <c r="N6">
+        <v>7.5187097812411327E-2</v>
+      </c>
+      <c r="O6">
+        <v>9.2178324540923715E-2</v>
+      </c>
+      <c r="P6">
+        <v>9.8520308812719781E-2</v>
+      </c>
+      <c r="Q6">
+        <v>2.0973295676043606E-2</v>
+      </c>
+      <c r="R6">
+        <v>2.6672789715633204E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7.2171323769520141E-3</v>
+      </c>
+      <c r="B7">
+        <v>0.20466432483092473</v>
+      </c>
+      <c r="C7">
+        <v>9.9999999895768271E-2</v>
+      </c>
+      <c r="D7">
+        <v>1568575537.3039272</v>
+      </c>
+      <c r="E7">
+        <v>15.38768594860198</v>
+      </c>
+      <c r="F7">
+        <v>72.176744142345981</v>
+      </c>
+      <c r="G7">
+        <v>0.58196438937078854</v>
+      </c>
+      <c r="H7">
+        <v>0.1637306187508428</v>
+      </c>
+      <c r="I7">
+        <v>4.1279696453638215E-8</v>
+      </c>
+      <c r="J7">
+        <v>5.0001376712519316E-3</v>
+      </c>
+      <c r="K7">
+        <v>0.99053303381537483</v>
+      </c>
+      <c r="L7">
+        <v>0.95949131454551995</v>
+      </c>
+      <c r="M7">
+        <v>0.98684624397295173</v>
+      </c>
+      <c r="N7">
+        <v>9.664803685865847E-2</v>
+      </c>
+      <c r="O7">
+        <v>0.19281575445191423</v>
+      </c>
+      <c r="P7">
+        <v>0.11168530097962748</v>
+      </c>
+      <c r="Q7">
+        <v>2.095401530746497E-2</v>
+      </c>
+      <c r="R7">
+        <v>2.6699257390410285E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.2725967521505301E-4</v>
+      </c>
+      <c r="B10">
+        <v>1.1993739194087553E-2</v>
+      </c>
+      <c r="C10">
+        <v>2.4552918518606016E-2</v>
+      </c>
+      <c r="D10">
+        <v>303200885.06844538</v>
+      </c>
+      <c r="E10">
+        <v>1.6192973300627467</v>
+      </c>
+      <c r="F10">
+        <v>2.7002248058917107</v>
+      </c>
+      <c r="G10">
+        <v>0.21319663172543957</v>
+      </c>
+      <c r="H10">
+        <v>1.663669593057689E-2</v>
+      </c>
+      <c r="I10">
+        <v>3.3027812666634468E-3</v>
+      </c>
+      <c r="J10">
+        <v>3.3333284952352165E-3</v>
+      </c>
+      <c r="K10">
+        <v>1.6463714510734249E-3</v>
+      </c>
+      <c r="L10">
+        <v>3.7194841128570279E-3</v>
+      </c>
+      <c r="M10">
+        <v>8.1010346831268017E-3</v>
+      </c>
+      <c r="N10">
+        <v>1.0864247817027092E-2</v>
+      </c>
+      <c r="O10">
+        <v>1.2756483123100756E-2</v>
+      </c>
+      <c r="P10">
+        <v>3.1298052001519007E-2</v>
+      </c>
+      <c r="Q10">
+        <v>4.8852209083045353E-4</v>
+      </c>
+      <c r="R10">
+        <v>2.5179500739234562E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.4738599434207719E-3</v>
+      </c>
+      <c r="B11">
+        <v>0.21677497345924515</v>
+      </c>
+      <c r="C11">
+        <v>2.4547279159958829E-2</v>
+      </c>
+      <c r="D11">
+        <v>326583444.34512126</v>
+      </c>
+      <c r="E11">
+        <v>5.4509860762583191</v>
+      </c>
+      <c r="F11">
+        <v>4.455262769280341</v>
+      </c>
+      <c r="G11">
+        <v>0.18653208822210188</v>
+      </c>
+      <c r="H11">
+        <v>0.17166136754163663</v>
+      </c>
+      <c r="I11">
+        <v>6.6602333795786044E-7</v>
+      </c>
+      <c r="J11">
+        <v>1.0708631790687299E-3</v>
+      </c>
+      <c r="K11">
+        <v>6.1587292917880557E-4</v>
+      </c>
+      <c r="L11">
+        <v>2.0829649505932534E-2</v>
+      </c>
+      <c r="M11">
+        <v>3.1689735417869021E-2</v>
+      </c>
+      <c r="N11">
+        <v>4.1502280322512136E-3</v>
+      </c>
+      <c r="O11">
+        <v>4.8416594032926287E-2</v>
+      </c>
+      <c r="P11">
+        <v>6.563828001184048E-2</v>
+      </c>
+      <c r="Q11">
+        <v>3.6735004728254622E-4</v>
+      </c>
+      <c r="R11">
+        <v>2.5671577619167341E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8.0834831872766671E-3</v>
+      </c>
+      <c r="B12">
+        <v>6.2168745082076066E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.1994584780844628E-2</v>
+      </c>
+      <c r="D12">
+        <v>225362239.38108262</v>
+      </c>
+      <c r="E12">
+        <v>3.3671168297151262</v>
+      </c>
+      <c r="F12">
+        <v>3.7935178192878136</v>
+      </c>
+      <c r="G12">
+        <v>0.10157683756220913</v>
+      </c>
+      <c r="H12">
+        <v>0.13287076105558546</v>
+      </c>
+      <c r="I12">
+        <v>1.1099206839491158E-3</v>
+      </c>
+      <c r="J12">
+        <v>1.491155448940396E-3</v>
+      </c>
+      <c r="K12">
+        <v>3.5487978199732939E-3</v>
+      </c>
+      <c r="L12">
+        <v>1.0159758260436006E-2</v>
+      </c>
+      <c r="M12">
+        <v>6.8300721229363993E-3</v>
+      </c>
+      <c r="N12">
+        <v>1.536814470265868E-2</v>
+      </c>
+      <c r="O12">
+        <v>2.8071907467135549E-2</v>
+      </c>
+      <c r="P12">
+        <v>2.1382863455327823E-2</v>
+      </c>
+      <c r="Q12">
+        <v>2.2890018555720107E-4</v>
+      </c>
+      <c r="R12">
+        <v>2.0299274734285723E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6.3360122857742784E-4</v>
+      </c>
+      <c r="B13">
+        <v>4.7271848244390062E-2</v>
+      </c>
+      <c r="C13">
+        <v>1.573185351950963E-2</v>
+      </c>
+      <c r="D13">
+        <v>548322859.71993709</v>
+      </c>
+      <c r="E13">
+        <v>4.9986682715416162</v>
+      </c>
+      <c r="F13">
+        <v>2.7618128074817472</v>
+      </c>
+      <c r="G13">
+        <v>0.19815659125126756</v>
+      </c>
+      <c r="H13">
+        <v>0.24646265996534966</v>
+      </c>
+      <c r="I13">
+        <v>2.4831981979158832E-3</v>
+      </c>
+      <c r="J13">
+        <v>2.8678135874797761E-3</v>
+      </c>
+      <c r="K13">
+        <v>1.1553948049722602E-3</v>
+      </c>
+      <c r="L13">
+        <v>7.6670951128889392E-3</v>
+      </c>
+      <c r="M13">
+        <v>1.4938257257636881E-2</v>
+      </c>
+      <c r="N13">
+        <v>9.8908396794604517E-3</v>
+      </c>
+      <c r="O13">
+        <v>2.8120269666226067E-2</v>
+      </c>
+      <c r="P13">
+        <v>4.263468782379095E-2</v>
+      </c>
+      <c r="Q13">
+        <v>4.7794254676021981E-4</v>
+      </c>
+      <c r="R13">
+        <v>3.7006385887008617E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.7730132747802112E-4</v>
+      </c>
+      <c r="B15">
+        <v>1.8238538900267456E-2</v>
+      </c>
+      <c r="C15">
+        <v>1.0420953683309997E-10</v>
+      </c>
+      <c r="D15">
+        <v>498176157.30909073</v>
+      </c>
+      <c r="E15">
+        <v>0.23560379063189529</v>
+      </c>
+      <c r="F15">
+        <v>2.9471882559705587</v>
+      </c>
+      <c r="G15">
+        <v>3.8190291770548557E-2</v>
+      </c>
+      <c r="H15">
+        <v>1.8804735994617402E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.1279664249079192E-8</v>
+      </c>
+      <c r="J15">
+        <v>4.9998623285380465E-3</v>
+      </c>
+      <c r="K15">
+        <v>1.095020593918139E-3</v>
+      </c>
+      <c r="L15">
+        <v>2.106934252323794E-2</v>
+      </c>
+      <c r="M15">
+        <v>5.2847381805418703E-3</v>
+      </c>
+      <c r="N15">
+        <v>5.6083414791154107E-3</v>
+      </c>
+      <c r="O15">
+        <v>5.4089587122424169E-2</v>
+      </c>
+      <c r="P15">
+        <v>2.3422468099408952E-2</v>
+      </c>
+      <c r="Q15">
+        <v>2.7126963587196205E-4</v>
+      </c>
+      <c r="R15">
+        <v>2.0695011051561837E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619B633D-6CFB-483C-9FB4-8F6342530738}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AQ23" sqref="AQ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12667,12 +13352,6 @@
       </c>
       <c r="X23" t="s">
         <v>169</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -13098,7 +13777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C81D8B5-6680-4FFB-85DD-B8A9C238D7F1}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>

</xml_diff>